<commit_message>
Minor updates to: README.txt TagsComments.xlsx: Added Examples to Tag explanation.
</commit_message>
<xml_diff>
--- a/TagsComments.xlsx
+++ b/TagsComments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="360" windowWidth="7980" windowHeight="5205"/>
+    <workbookView xWindow="720" yWindow="360" windowWidth="7980" windowHeight="5205" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Count" sheetId="9" r:id="rId1"/>
@@ -38,6 +38,19 @@
           <t>برتقالي: فيه شك
 أحمر: خاطئ ويُلغى
 أخضر: يُضاف</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>Examples are copied from dictStems verbatim.</t>
         </r>
       </text>
     </comment>
@@ -212,7 +225,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="526">
   <si>
     <t>Nprop</t>
   </si>
@@ -1507,12 +1520,450 @@
   <si>
     <t>StemCount</t>
   </si>
+  <si>
+    <t>Examples</t>
+  </si>
+  <si>
+    <t>اُتْرُك,اِسْتَخْدِم,كُل</t>
+  </si>
+  <si>
+    <t>قُل,كُن</t>
+  </si>
+  <si>
+    <t>اِتَّصِل</t>
+  </si>
+  <si>
+    <t>بْتَعِث,بْتَعِد,بْحَث,تَأَبَّط,تَبايَع,حْتَرِف,رْأَس,سْتَوْدِع,نْتَصِح</t>
+  </si>
+  <si>
+    <t>بْتَغَى,بْتَنَى,هْوَى</t>
+  </si>
+  <si>
+    <t>أْبَى,أْوَى,أْوَى</t>
+  </si>
+  <si>
+    <t>بَكَّى,بْتَلَى,ؤاسَى</t>
+  </si>
+  <si>
+    <t>بْتَغِي,حْتَمِي,حْذُو,هْفُو,هْمُو</t>
+  </si>
+  <si>
+    <t>أْلُو,أْوِي</t>
+  </si>
+  <si>
+    <t>بَكِّي,رْضِي,رْعِي</t>
+  </si>
+  <si>
+    <t>بْتَن,بْن,بْهَ,تَساو,هْوَ</t>
+  </si>
+  <si>
+    <t>أْذَ,أْو</t>
+  </si>
+  <si>
+    <t>بَكّ,رَبّ,رَدّ,ؤاس</t>
+  </si>
+  <si>
+    <t>نْتَوَى</t>
+  </si>
+  <si>
+    <t>بْقَي,تَسَنَّي,وْهَي</t>
+  </si>
+  <si>
+    <t>أْبَي,أْذَي,أْسَي</t>
+  </si>
+  <si>
+    <t>بادَي,بارَي,جَلَّي</t>
+  </si>
+  <si>
+    <t>تَوَفَّ</t>
+  </si>
+  <si>
+    <t>أْزِز,بِع,سْتَغْشِش,ئِن</t>
+  </si>
+  <si>
+    <t>بُر,تَراصِص,سْتَقِم</t>
+  </si>
+  <si>
+    <t>دْلِل</t>
+  </si>
+  <si>
+    <t>بَت,حَط,حَق,هَل</t>
+  </si>
+  <si>
+    <t>بِت,رِع</t>
+  </si>
+  <si>
+    <t>سْتَجْنِن,سْتَنِن</t>
+  </si>
+  <si>
+    <t>سْتَكْنِن,طْمَأْنِن</t>
+  </si>
+  <si>
+    <t>تَأَسّا,تَمادا,تَمارا,هْوا</t>
+  </si>
+  <si>
+    <t>أْبا,أْبا</t>
+  </si>
+  <si>
+    <t>تَكَأْكَؤ,تَلَأْلَؤ</t>
+  </si>
+  <si>
+    <t>أْنُث,تَأَقْلَم,صِد,كْرُه,وْقُر,يْقُظ</t>
+  </si>
+  <si>
+    <t>بَتِّل,حَصْحِص,ياسِر</t>
+  </si>
+  <si>
+    <t>تَزِر,مُر</t>
+  </si>
+  <si>
+    <t>وثِر,ونِق</t>
+  </si>
+  <si>
+    <t>أْجُر,أْوَد</t>
+  </si>
+  <si>
+    <t>ؤْثِر,ؤْنِق</t>
+  </si>
+  <si>
+    <t>نْتَقَد</t>
+  </si>
+  <si>
+    <t>بَتَّت,غْرَز,ؤَيَّض</t>
+  </si>
+  <si>
+    <t>بِيع,تِمّ,ئِين</t>
+  </si>
+  <si>
+    <t>بَرّ,هْتاج</t>
+  </si>
+  <si>
+    <t>أَثّ</t>
+  </si>
+  <si>
+    <t>حِظّ,ماسّ</t>
+  </si>
+  <si>
+    <t>أْتَمّ</t>
+  </si>
+  <si>
+    <t>بات,هان</t>
+  </si>
+  <si>
+    <t>بِحّ,وادّ</t>
+  </si>
+  <si>
+    <t>تَباطَؤ,وبَؤ</t>
+  </si>
+  <si>
+    <t>فِيؤ</t>
+  </si>
+  <si>
+    <t>ضِيؤ,فَيِّؤ,هايِؤ</t>
+  </si>
+  <si>
+    <t>تَرَدَّئ,وبُئ</t>
+  </si>
+  <si>
+    <t>فِيئ</t>
+  </si>
+  <si>
+    <t>تَوَفّ</t>
+  </si>
+  <si>
+    <t>رائ,سِيئ</t>
+  </si>
+  <si>
+    <t>بَرْعِم,تَوِّه,فَسِّح,يَوِّد</t>
+  </si>
+  <si>
+    <t>بْدَآ,نْكَآ</t>
+  </si>
+  <si>
+    <t>تَبايَن</t>
+  </si>
+  <si>
+    <t>حْسُن,يْمُن</t>
+  </si>
+  <si>
+    <t>أْذَن,أْمُن</t>
+  </si>
+  <si>
+    <t>ؤْذِن,ؤْمِن</t>
+  </si>
+  <si>
+    <t>بَن,بْطَن,تْقَن,دَخَّن,وهَن</t>
+  </si>
+  <si>
+    <t>حَسِّن,نْتِن</t>
+  </si>
+  <si>
+    <t>اِسْتِيراد,اِنْتِهاك,إِيران,أَتْراك,أَحْلاق,بَسكَوِيت,بَشَر,بِكْر,شُهُب,شُهُود,فَسْح,نَحْو,ياسْمِين</t>
+  </si>
+  <si>
+    <t>إِنْجاص,إِنْسان,ذَكِيّ,كاتِب</t>
+  </si>
+  <si>
+    <t>لَذِيذ,لائِم</t>
+  </si>
+  <si>
+    <t>اِبْيِضاض,اِتِّساق,اِسْتِظْهار,اِسْتِظْهار,اِكْتِظاظ,تَلْوِين,وُقُوع</t>
+  </si>
+  <si>
+    <t>لِتْر,لِحام,لِيتْر,لانْش</t>
+  </si>
+  <si>
+    <t>لَبْث,لَبْس,لاوَعْي</t>
+  </si>
+  <si>
+    <t>أَبْطَآ,أَصْدَآ,نَبَآ</t>
+  </si>
+  <si>
+    <t>مُبْتَدَ,هَيْ</t>
+  </si>
+  <si>
+    <t>اِبْتِسام,إِبْراهِيم,أَرِيحا,أُمَم,بَهْبَهانِي,راجِح,عَبْداللّه,هُونْدا</t>
+  </si>
+  <si>
+    <t>لِوَى,لاوُوس</t>
+  </si>
+  <si>
+    <t>اِبْتِداء,أَسْواء,قَضاء,مُسْتَوِي</t>
+  </si>
+  <si>
+    <t>لَدّاء,لُوبِياء,لُؤَماء,لُؤْلُؤ</t>
+  </si>
+  <si>
+    <t>حَشايا,حَظايا,حَلا,هَدايا</t>
+  </si>
+  <si>
+    <t>أَب,أَخ,بَدْء,بَرْء,بانِي,خالِي,رامِي,واقِي</t>
+  </si>
+  <si>
+    <t>حامِي,شارِي,مُرَبِّي,والِي</t>
+  </si>
+  <si>
+    <t>اِبْتِداعِيّ,بَحّار,بَيْطَرِيّ,حَبَشِيّ,دانِمارْكِيّ,عاقّ,مَخْلُوط,مُتَذَوِّق,مُعَثِّر,هَدّاف</t>
+  </si>
+  <si>
+    <t>لااِجْتِماعِيّ,لااِجْتِماعِيّ,لاجِئ,لائِق</t>
+  </si>
+  <si>
+    <t>اِبْتِغاء,اِسْتِدْعاء,إِحْصاء,أُولَي,عاصِي,مُلْتَوَي</t>
+  </si>
+  <si>
+    <t>لَوْز,لُؤْلُؤ,لِقاء,لاغِي</t>
+  </si>
+  <si>
+    <t>اِسْتِبْدادِيّ,اِسْتِراح,إِخْو,إِلْزامِيّ,إِمات,بَغْثَر,جَنادِر,زُهْر,صُفْر,كُدْر,مَكْرَه</t>
+  </si>
+  <si>
+    <t>اِحْتِمالِيّ,شَمْسِيّ,شَهِيد,شِراعِيّ,غَرِيب</t>
+  </si>
+  <si>
+    <t>لَأْلَأ</t>
+  </si>
+  <si>
+    <t>لَبِق,لَسِن,لَصِق,لاهُوتِيّ</t>
+  </si>
+  <si>
+    <t>اِبْتِسام,اِسْتِغاث,إِثار,بِذْر,حَسَن,دَوّاس,صارِي,مَجان</t>
+  </si>
+  <si>
+    <t>لَبِن,لَوْح,لاهِي</t>
+  </si>
+  <si>
+    <t>إِجّاص,إِفاد,أَرَض,حُفْر,سِدار,وَصِيّ</t>
+  </si>
+  <si>
+    <t>لَزْم,لاحِق,لافِت</t>
+  </si>
+  <si>
+    <t>اِبْتِكار,اِتِّحاد,اِسْتِرْضاء,تَقَصِّي,رَكَل,صَرْفِيّ,لَفَظ,نَفَث,ياء</t>
+  </si>
+  <si>
+    <t>لَبَن,لَعَن,لافِت</t>
+  </si>
+  <si>
+    <t>اِبْتِدائ,اِحْتِذائ,اِعْتِنائ,مِينائ</t>
+  </si>
+  <si>
+    <t>إِبْلِيس,إِسْحاق,إِسْرائِيل,أَحادِيث,أَقاوِيل,خَواتِيم,مَباخِر,مَعاقِل,يَنابِيع</t>
+  </si>
+  <si>
+    <t>لَآلِئ,لَفائِف,لَوائِح</t>
+  </si>
+  <si>
+    <t>اِبْتِكار,اِبْن,اِتِّهام,اِتِّهام,إِزْمِيل,بُنْدُق,خَطَر,سَرْج</t>
+  </si>
+  <si>
+    <t>لَحْد,لَفْظ,لَقَب</t>
+  </si>
+  <si>
+    <t>اِبْتِذال,تَأْوِيل,مُفْتَرَق</t>
+  </si>
+  <si>
+    <t>لُورْد,لاقِط,لام</t>
+  </si>
+  <si>
+    <t>أَخْيَر,أَفْوَه,أَكْرَم,آلَف,آلَم</t>
+  </si>
+  <si>
+    <t>اِتِّباع,تَبَع,جُوع,طَوِيل</t>
+  </si>
+  <si>
+    <t>قَيْئ,وَضِيئ</t>
+  </si>
+  <si>
+    <t>اِبْتِغاؤ,إِرْضاؤ,عُواؤ</t>
+  </si>
+  <si>
+    <t>لَأْلاؤ</t>
+  </si>
+  <si>
+    <t>عَدّائ,وَشّائ</t>
+  </si>
+  <si>
+    <t>سَقّاؤ,وَشّاؤ</t>
+  </si>
+  <si>
+    <t>اِتِّكائ,نُزَلائ,نُها,يُسْرا</t>
+  </si>
+  <si>
+    <t>لَدْغا,لِحائ,لِقائ</t>
+  </si>
+  <si>
+    <t>أَحاج,باغ,باغ,تَساو,طاه,مَدار,واق</t>
+  </si>
+  <si>
+    <t>اِنْتِصار,إِخْلاص,إِلِكْترِيك,إِياد,إِياد,بِيرل,ماكْدُونالْدز</t>
+  </si>
+  <si>
+    <t>أَرْبَع,عِشْر</t>
+  </si>
+  <si>
+    <t>أَقْدَم,آخَر,خال,شاد,مُسْتَعْص</t>
+  </si>
+  <si>
+    <t>لِد,لاه</t>
+  </si>
+  <si>
+    <t>اِبْتَدَر,اِسْتَشْرَف,اِسْتَشْرَف,اِنْتَخَب,أَرْبَح,تَرَحَّب,جَصَّص,صَدَّق,ناهَز</t>
+  </si>
+  <si>
+    <t>اِبْتَغَى,أَخْلَى,وَصَّى</t>
+  </si>
+  <si>
+    <t>جَفا,شَكا,هَجا</t>
+  </si>
+  <si>
+    <t>اِزْدَهَي,أَجْرَي,قاضَي</t>
+  </si>
+  <si>
+    <t>اِبْتَع,اِسْتَحْبَب,قُل</t>
+  </si>
+  <si>
+    <t>اِرْتَح,عَزَز</t>
+  </si>
+  <si>
+    <t>سُلَل,غُمِم</t>
+  </si>
+  <si>
+    <t>اِسْتَدَن,كَنَن</t>
+  </si>
+  <si>
+    <t>اِزْدَن,اِسْتَكَن</t>
+  </si>
+  <si>
+    <t>اِسْتَمَت,مُت</t>
+  </si>
+  <si>
+    <t>اِنْبَتَت</t>
+  </si>
+  <si>
+    <t>اِبْتَنا,اِسْتَخْفا,اِمْتَطا,آذا,تَناسا,نَحا</t>
+  </si>
+  <si>
+    <t>اِبْتَأَس,اِسْتَنْكَر,أَعْوَز,تَجَمَّد,سَبَخ,قَصُر</t>
+  </si>
+  <si>
+    <t>بَقِي,نَسِي</t>
+  </si>
+  <si>
+    <t>خَفِي,سَخِي</t>
+  </si>
+  <si>
+    <t>تُوُفِّي</t>
+  </si>
+  <si>
+    <t>اُتُّفِق,سُمِع</t>
+  </si>
+  <si>
+    <t>أُغْمِي,غُشِي,غُمِي</t>
+  </si>
+  <si>
+    <t>اُسْتُعِير,نُهِي</t>
+  </si>
+  <si>
+    <t>اِتَّق,اِسْتَسْق,تَرَوّ,غَطّ</t>
+  </si>
+  <si>
+    <t>اِسْتَصْب,صَف,واس</t>
+  </si>
+  <si>
+    <t>اِبْتاع,اِسْتَجار,اِسْتَجار,أَعان,دان,هَمّ</t>
+  </si>
+  <si>
+    <t>اِخْتال,ذاب</t>
+  </si>
+  <si>
+    <t>أُتِيح,بيع</t>
+  </si>
+  <si>
+    <t>اُسْتُفِيد,اُسْتُفِيد</t>
+  </si>
+  <si>
+    <t>اِخْتَبَؤ,هَدَؤ,هَدَّؤ</t>
+  </si>
+  <si>
+    <t>اِسْتَدْفَؤ,بَه,حَل</t>
+  </si>
+  <si>
+    <t>تُوُفّ</t>
+  </si>
+  <si>
+    <t>اِتَّكَآ,اِسْتَقْرَآ,اِسْتَقْرَآ,لَجَّآ,هَدَآ</t>
+  </si>
+  <si>
+    <t>اِجْتَرَآ,تَوَضَّآ,نَبَآ</t>
+  </si>
+  <si>
+    <t>أَبْدَأ,أَنْبَأ,ظَمَّأ</t>
+  </si>
+  <si>
+    <t>اِسْتَدْفَأ,تَجَزَّأ,تَخَبَّأ,هَنَأ</t>
+  </si>
+  <si>
+    <t>اِحْتَجَن,تَحَسَّن,يَمَّن</t>
+  </si>
+  <si>
+    <t>اِقْتَرَن,تَزَيَّن</t>
+  </si>
+  <si>
+    <t>قُورِن</t>
+  </si>
+  <si>
+    <t>اِسْتَلْفَت,أَثْبَت,باغَت,نَحَت,وَقَّت</t>
+  </si>
+  <si>
+    <t>اِخْتَفَت,مَقُت</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="30">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1749,8 +2200,22 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="40">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1932,20 +2397,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="22"/>
-        <bgColor indexed="0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="0"/>
       </patternFill>
     </fill>
     <fill>
@@ -1972,8 +2425,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -2090,21 +2549,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="22"/>
       </left>
       <right style="thin">
@@ -2173,7 +2617,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" readingOrder="2"/>
@@ -2184,21 +2628,15 @@
     <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2210,28 +2648,28 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="38" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2241,16 +2679,16 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="39" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2259,10 +2697,9 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -2272,18 +2709,19 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2628,7 +3066,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -2643,7 +3081,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="4">
@@ -2651,7 +3089,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="4">
@@ -2659,7 +3097,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="4">
@@ -2667,7 +3105,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4">
@@ -2675,7 +3113,7 @@
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="4">
@@ -2683,7 +3121,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="30">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="4">
@@ -2691,7 +3129,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" ht="30">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B8" s="4">
@@ -2699,7 +3137,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" ht="30">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B9" s="4">
@@ -2707,7 +3145,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="30">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="7" t="s">
         <v>52</v>
       </c>
       <c r="B10" s="4">
@@ -2715,7 +3153,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="30">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="7" t="s">
         <v>50</v>
       </c>
       <c r="B11" s="4">
@@ -2723,7 +3161,7 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="4">
@@ -2731,7 +3169,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" ht="30">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B13" s="4">
@@ -2739,7 +3177,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="30">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B14" s="4">
@@ -2747,7 +3185,7 @@
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B15" s="4">
@@ -2755,7 +3193,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="30">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="7" t="s">
         <v>57</v>
       </c>
       <c r="B16" s="4">
@@ -2763,7 +3201,7 @@
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B17" s="4">
@@ -2771,7 +3209,7 @@
       </c>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="7" t="s">
         <v>93</v>
       </c>
       <c r="B18" s="4">
@@ -2779,7 +3217,7 @@
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="7" t="s">
         <v>94</v>
       </c>
       <c r="B19" s="4">
@@ -2787,7 +3225,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="30">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="7" t="s">
         <v>106</v>
       </c>
       <c r="B20" s="4">
@@ -2795,7 +3233,7 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="7" t="s">
         <v>73</v>
       </c>
       <c r="B21" s="4">
@@ -2803,7 +3241,7 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="4">
@@ -2811,7 +3249,7 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="4">
@@ -2819,7 +3257,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="30">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B24" s="4">
@@ -2827,7 +3265,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" ht="30">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="7" t="s">
         <v>88</v>
       </c>
       <c r="B25" s="4">
@@ -2835,7 +3273,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="30">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="7" t="s">
         <v>107</v>
       </c>
       <c r="B26" s="4">
@@ -2843,7 +3281,7 @@
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B27" s="4">
@@ -2851,7 +3289,7 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="7" t="s">
         <v>96</v>
       </c>
       <c r="B28" s="4">
@@ -2859,7 +3297,7 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="7" t="s">
         <v>95</v>
       </c>
       <c r="B29" s="4">
@@ -2867,7 +3305,7 @@
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="7" t="s">
         <v>72</v>
       </c>
       <c r="B30" s="4">
@@ -2875,7 +3313,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="45">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="7" t="s">
         <v>103</v>
       </c>
       <c r="B31" s="4">
@@ -2883,7 +3321,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" ht="30">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="19" t="s">
         <v>105</v>
       </c>
       <c r="B32" s="4">
@@ -2891,7 +3329,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="45">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B33" s="4">
@@ -2899,7 +3337,7 @@
       </c>
     </row>
     <row r="34" spans="1:2" ht="30">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="7" t="s">
         <v>116</v>
       </c>
       <c r="B34" s="4">
@@ -2907,7 +3345,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="30">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="7" t="s">
         <v>117</v>
       </c>
       <c r="B35" s="4">
@@ -2915,7 +3353,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" ht="45">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B36" s="4">
@@ -2923,7 +3361,7 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="45">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B37" s="4">
@@ -2931,7 +3369,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="45">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="7" t="s">
         <v>63</v>
       </c>
       <c r="B38" s="4">
@@ -2939,7 +3377,7 @@
       </c>
     </row>
     <row r="39" spans="1:2" ht="30">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="7" t="s">
         <v>65</v>
       </c>
       <c r="B39" s="4">
@@ -2947,7 +3385,7 @@
       </c>
     </row>
     <row r="40" spans="1:2" ht="30">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="7" t="s">
         <v>69</v>
       </c>
       <c r="B40" s="4">
@@ -2955,7 +3393,7 @@
       </c>
     </row>
     <row r="41" spans="1:2" ht="30">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B41" s="4">
@@ -2963,15 +3401,15 @@
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="18" t="s">
+      <c r="A42" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="B42" s="19">
+      <c r="B42" s="17">
         <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="45">
-      <c r="A43" s="9" t="s">
+      <c r="A43" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B43" s="4">
@@ -2979,7 +3417,7 @@
       </c>
     </row>
     <row r="44" spans="1:2" ht="30">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="7" t="s">
         <v>124</v>
       </c>
       <c r="B44" s="4">
@@ -2987,7 +3425,7 @@
       </c>
     </row>
     <row r="45" spans="1:2" ht="45">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="7" t="s">
         <v>70</v>
       </c>
       <c r="B45" s="4">
@@ -2995,7 +3433,7 @@
       </c>
     </row>
     <row r="46" spans="1:2" ht="30">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="7" t="s">
         <v>85</v>
       </c>
       <c r="B46" s="4">
@@ -3003,7 +3441,7 @@
       </c>
     </row>
     <row r="47" spans="1:2" ht="45">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="7" t="s">
         <v>59</v>
       </c>
       <c r="B47" s="4">
@@ -3011,7 +3449,7 @@
       </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="7" t="s">
         <v>133</v>
       </c>
       <c r="B48" s="4">
@@ -3019,7 +3457,7 @@
       </c>
     </row>
     <row r="49" spans="1:2" ht="30">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B49" s="4">
@@ -3027,7 +3465,7 @@
       </c>
     </row>
     <row r="50" spans="1:2">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="7" t="s">
         <v>115</v>
       </c>
       <c r="B50" s="4">
@@ -3035,15 +3473,15 @@
       </c>
     </row>
     <row r="51" spans="1:2" ht="30">
-      <c r="A51" s="18" t="s">
+      <c r="A51" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="B51" s="19">
+      <c r="B51" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="30">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="7" t="s">
         <v>129</v>
       </c>
       <c r="B52" s="4">
@@ -3051,7 +3489,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" ht="30">
-      <c r="A53" s="21" t="s">
+      <c r="A53" s="19" t="s">
         <v>128</v>
       </c>
       <c r="B53" s="4">
@@ -3059,15 +3497,15 @@
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="14" t="s">
+      <c r="A54" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="B54" s="15">
+      <c r="B54" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="30">
-      <c r="A55" s="9" t="s">
+      <c r="A55" s="7" t="s">
         <v>157</v>
       </c>
       <c r="B55" s="4">
@@ -3075,7 +3513,7 @@
       </c>
     </row>
     <row r="56" spans="1:2" ht="30">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="7" t="s">
         <v>154</v>
       </c>
       <c r="B56" s="4">
@@ -3083,10 +3521,10 @@
       </c>
     </row>
     <row r="57" spans="1:2" ht="30">
-      <c r="A57" s="14" t="s">
+      <c r="A57" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="B57" s="15">
+      <c r="B57" s="13">
         <v>1</v>
       </c>
     </row>
@@ -3108,36 +3546,49 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K166"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E133" sqref="E133"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="22.5"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="12" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" style="10" customWidth="1"/>
     <col min="2" max="2" width="4.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="75" style="12" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="32" customWidth="1"/>
-    <col min="5" max="6" width="9.140625" style="23"/>
-    <col min="7" max="7" width="9.140625" style="23" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="23" customWidth="1"/>
-    <col min="9" max="11" width="9.140625" style="23"/>
+    <col min="3" max="3" width="75" style="10" customWidth="1"/>
+    <col min="4" max="4" width="48.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" style="21" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="21"/>
+    <col min="7" max="7" width="9.140625" style="21" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="21" customWidth="1"/>
+    <col min="9" max="11" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.5">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:11" ht="18.75">
+      <c r="A1" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="37" t="s">
         <v>339</v>
       </c>
-      <c r="D1" s="23"/>
-    </row>
-    <row r="2" spans="1:4" ht="45">
-      <c r="A2" s="9" t="s">
+      <c r="D1" s="37" t="s">
+        <v>380</v>
+      </c>
+      <c r="E1" s="37"/>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="J1"/>
+      <c r="K1"/>
+    </row>
+    <row r="2" spans="1:11" ht="45">
+      <c r="A2" s="7" t="s">
         <v>66</v>
       </c>
       <c r="B2" s="4">
@@ -3146,10 +3597,12 @@
       <c r="C2" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="D2" s="23"/>
-    </row>
-    <row r="3" spans="1:4" ht="45">
-      <c r="A3" s="9" t="s">
+      <c r="D2" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="45">
+      <c r="A3" s="7" t="s">
         <v>125</v>
       </c>
       <c r="B3" s="4">
@@ -3158,10 +3611,12 @@
       <c r="C3" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="D3" s="23"/>
-    </row>
-    <row r="4" spans="1:4" ht="45">
-      <c r="A4" s="9" t="s">
+      <c r="D3" s="2" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="45">
+      <c r="A4" s="7" t="s">
         <v>155</v>
       </c>
       <c r="B4" s="4">
@@ -3170,10 +3625,12 @@
       <c r="C4" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="D4" s="23"/>
-    </row>
-    <row r="5" spans="1:4" ht="67.5">
-      <c r="A5" s="9" t="s">
+      <c r="D4" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="67.5">
+      <c r="A5" s="7" t="s">
         <v>132</v>
       </c>
       <c r="B5" s="4">
@@ -3182,10 +3639,9 @@
       <c r="C5" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D5" s="23"/>
-    </row>
-    <row r="6" spans="1:4" ht="67.5">
-      <c r="A6" s="9" t="s">
+    </row>
+    <row r="6" spans="1:11" ht="67.5">
+      <c r="A6" s="7" t="s">
         <v>126</v>
       </c>
       <c r="B6" s="4">
@@ -3194,140 +3650,139 @@
       <c r="C6" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D6" s="23"/>
-    </row>
-    <row r="7" spans="1:4" ht="22.5">
-      <c r="A7" s="9" t="s">
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="7" t="s">
         <v>82</v>
       </c>
       <c r="B7" s="4">
         <v>134</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="D7" s="23" t="str">
+      <c r="D7" s="2" t="str">
         <f>LEFT(C7,4)</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="22.5">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:11">
+      <c r="A8" s="7" t="s">
         <v>61</v>
       </c>
       <c r="B8" s="4">
         <v>682</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="23" t="str">
+      <c r="D8" s="2" t="str">
         <f t="shared" ref="D8:D16" si="0">LEFT(C8,4)</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="22.5">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:11">
+      <c r="A9" s="7" t="s">
         <v>62</v>
       </c>
       <c r="B9" s="4">
         <v>64</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="D9" s="23" t="str">
+      <c r="D9" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="22.5">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:11">
+      <c r="A10" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="4">
         <v>149</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="D10" s="23" t="str">
+      <c r="D10" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="22.5">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:11">
+      <c r="A11" s="7" t="s">
         <v>77</v>
       </c>
       <c r="B11" s="4">
         <v>45</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="23" t="str">
+      <c r="D11" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="22.5">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:11">
+      <c r="A12" s="7" t="s">
         <v>127</v>
       </c>
       <c r="B12" s="4">
         <v>3</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="23" t="str">
+      <c r="D12" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="22.5">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:11">
+      <c r="A13" s="7" t="s">
         <v>87</v>
       </c>
       <c r="B13" s="4">
         <v>11</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="23" t="str">
+      <c r="D13" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="34.5">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:11" ht="34.5">
+      <c r="A14" s="7" t="s">
         <v>86</v>
       </c>
       <c r="B14" s="4">
         <v>17</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="23" t="str">
+      <c r="D14" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="22.5">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:11">
+      <c r="A15" s="7" t="s">
         <v>78</v>
       </c>
       <c r="B15" s="4">
         <v>34</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="D15" s="23" t="str">
+      <c r="D15" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="22.5">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:11">
+      <c r="A16" s="7" t="s">
         <v>84</v>
       </c>
       <c r="B16" s="4">
         <v>8</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="23" t="str">
+      <c r="D16" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:9" ht="67.5">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="4">
@@ -3336,12 +3791,14 @@
       <c r="C17" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="D17" s="23"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
+      <c r="D17" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
     </row>
     <row r="18" spans="1:9" ht="67.5">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="4">
@@ -3350,13 +3807,15 @@
       <c r="C18" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="D18" s="23"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
+      <c r="D18" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
     </row>
     <row r="19" spans="1:9" ht="45">
-      <c r="A19" s="9" t="s">
+      <c r="A19" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B19" s="4">
@@ -3365,13 +3824,15 @@
       <c r="C19" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="D19" s="23"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
+      <c r="D19" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
     </row>
     <row r="20" spans="1:9" ht="67.5">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="7" t="s">
         <v>49</v>
       </c>
       <c r="B20" s="4">
@@ -3380,27 +3841,28 @@
       <c r="C20" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="D20" s="23"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
+      <c r="D20" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
     </row>
     <row r="21" spans="1:9" ht="34.5">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="13">
         <v>1</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="D21" s="23"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="I21" s="24"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="I21" s="22"/>
     </row>
     <row r="22" spans="1:9" ht="45">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="7" t="s">
         <v>52</v>
       </c>
       <c r="B22" s="4">
@@ -3409,14 +3871,17 @@
       <c r="C22" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="D22" s="23"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
+      <c r="D22" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
     </row>
     <row r="23" spans="1:9" ht="49.5">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="7" t="s">
         <v>46</v>
       </c>
       <c r="B23" s="4">
@@ -3425,13 +3890,16 @@
       <c r="C23" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="D23" s="23"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="I23" s="24"/>
+      <c r="D23" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="E23"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="I23" s="22"/>
     </row>
     <row r="24" spans="1:9" ht="45">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B24" s="4">
@@ -3440,69 +3908,84 @@
       <c r="C24" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="D24" s="23"/>
-      <c r="G24" s="24"/>
-      <c r="I24" s="24"/>
+      <c r="D24" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="E24"/>
+      <c r="G24" s="22"/>
+      <c r="I24" s="22"/>
     </row>
     <row r="25" spans="1:9" ht="67.5">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="7" t="s">
         <v>41</v>
       </c>
       <c r="B25" s="4">
         <v>640</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="11" t="s">
         <v>358</v>
       </c>
-      <c r="D25" s="23"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
+      <c r="D25" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="E25"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
     </row>
     <row r="26" spans="1:9" ht="112.5">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="7" t="s">
         <v>37</v>
       </c>
       <c r="B26" s="4">
         <v>16</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="11" t="s">
         <v>365</v>
       </c>
-      <c r="D26" s="23"/>
-      <c r="G26" s="24"/>
-      <c r="I26" s="24"/>
+      <c r="D26" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="E26"/>
+      <c r="G26" s="22"/>
+      <c r="I26" s="22"/>
     </row>
     <row r="27" spans="1:9" ht="112.5">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B27" s="4">
         <v>314</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="11" t="s">
         <v>357</v>
       </c>
-      <c r="D27" s="23"/>
-      <c r="G27" s="24"/>
+      <c r="D27" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="E27"/>
+      <c r="G27" s="22"/>
     </row>
     <row r="28" spans="1:9" ht="34.5">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="B28" s="15">
+      <c r="B28" s="13">
         <v>1</v>
       </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="D28" s="23"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
+      <c r="D28" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="E28"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
     </row>
     <row r="29" spans="1:9" ht="67.5">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="7" t="s">
         <v>40</v>
       </c>
       <c r="B29" s="4">
@@ -3511,13 +3994,16 @@
       <c r="C29" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="D29" s="23"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
+      <c r="D29" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="E29"/>
+      <c r="G29" s="22"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="22"/>
     </row>
     <row r="30" spans="1:9" ht="45">
-      <c r="A30" s="9" t="s">
+      <c r="A30" s="7" t="s">
         <v>36</v>
       </c>
       <c r="B30" s="4">
@@ -3526,11 +4012,14 @@
       <c r="C30" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="D30" s="23"/>
-      <c r="G30" s="24"/>
+      <c r="D30" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="E30"/>
+      <c r="G30" s="22"/>
     </row>
     <row r="31" spans="1:9" ht="67.5">
-      <c r="A31" s="9" t="s">
+      <c r="A31" s="7" t="s">
         <v>50</v>
       </c>
       <c r="B31" s="4">
@@ -3539,39 +4028,48 @@
       <c r="C31" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="G31" s="24"/>
-    </row>
-    <row r="32" spans="1:9" s="23" customFormat="1" ht="45">
-      <c r="A32" s="21" t="s">
+      <c r="D31" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="E31"/>
+      <c r="G31" s="22"/>
+    </row>
+    <row r="32" spans="1:9" s="21" customFormat="1" ht="45">
+      <c r="A32" s="19" t="s">
         <v>157</v>
       </c>
       <c r="B32" s="4">
         <v>1</v>
       </c>
-      <c r="C32" s="38" t="s">
+      <c r="C32" s="35" t="s">
         <v>360</v>
       </c>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="I32" s="24"/>
-    </row>
-    <row r="33" spans="1:10" s="23" customFormat="1" ht="45">
-      <c r="A33" s="23" t="s">
+      <c r="D32" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="E32"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="I32" s="22"/>
+    </row>
+    <row r="33" spans="1:10" s="21" customFormat="1" ht="45">
+      <c r="A33" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B33" s="4">
         <v>1</v>
       </c>
-      <c r="C33" s="38" t="s">
+      <c r="C33" s="35" t="s">
         <v>361</v>
       </c>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="I33" s="24"/>
+      <c r="D33" s="2"/>
+      <c r="E33"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="I33" s="22"/>
     </row>
     <row r="34" spans="1:10" ht="67.5">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B34" s="4">
@@ -3580,13 +4078,16 @@
       <c r="C34" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="D34" s="23"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="I34" s="24"/>
+      <c r="D34" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="E34"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="I34" s="22"/>
     </row>
     <row r="35" spans="1:10" ht="67.5">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="7" t="s">
         <v>58</v>
       </c>
       <c r="B35" s="4">
@@ -3595,13 +4096,16 @@
       <c r="C35" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="D35" s="23"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="I35" s="24"/>
+      <c r="D35" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="E35"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="I35" s="22"/>
     </row>
     <row r="36" spans="1:10" ht="67.5">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="7" t="s">
         <v>117</v>
       </c>
       <c r="B36" s="4">
@@ -3610,12 +4114,15 @@
       <c r="C36" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="D36" s="23"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
+      <c r="D36" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="E36"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
     </row>
     <row r="37" spans="1:10" ht="67.5">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="7" t="s">
         <v>107</v>
       </c>
       <c r="B37" s="4">
@@ -3624,13 +4131,16 @@
       <c r="C37" s="3" t="s">
         <v>314</v>
       </c>
-      <c r="D37" s="23"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="I37" s="24"/>
+      <c r="D37" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="E37"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="I37" s="22"/>
     </row>
     <row r="38" spans="1:10" ht="67.5">
-      <c r="A38" s="9" t="s">
+      <c r="A38" s="7" t="s">
         <v>94</v>
       </c>
       <c r="B38" s="4">
@@ -3639,13 +4149,16 @@
       <c r="C38" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="D38" s="23"/>
-      <c r="G38" s="24"/>
-      <c r="I38" s="24"/>
-      <c r="J38" s="24"/>
+      <c r="D38" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="E38"/>
+      <c r="G38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
     </row>
     <row r="39" spans="1:10" ht="67.5">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="7" t="s">
         <v>115</v>
       </c>
       <c r="B39" s="4">
@@ -3654,13 +4167,16 @@
       <c r="C39" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="D39" s="23"/>
-      <c r="G39" s="24"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24"/>
+      <c r="D39" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="E39"/>
+      <c r="G39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="22"/>
     </row>
     <row r="40" spans="1:10" ht="67.5">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="7" t="s">
         <v>124</v>
       </c>
       <c r="B40" s="4">
@@ -3669,13 +4185,16 @@
       <c r="C40" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="D40" s="23"/>
-      <c r="G40" s="24"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24"/>
+      <c r="D40" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E40"/>
+      <c r="G40" s="22"/>
+      <c r="I40" s="22"/>
+      <c r="J40" s="22"/>
     </row>
     <row r="41" spans="1:10" ht="67.5">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B41" s="4">
@@ -3684,13 +4203,16 @@
       <c r="C41" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="D41" s="23"/>
-      <c r="G41" s="24"/>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24"/>
+      <c r="D41" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E41"/>
+      <c r="G41" s="22"/>
+      <c r="I41" s="22"/>
+      <c r="J41" s="22"/>
     </row>
     <row r="42" spans="1:10" ht="67.5">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="7" t="s">
         <v>35</v>
       </c>
       <c r="B42" s="4">
@@ -3699,24 +4221,30 @@
       <c r="C42" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="D42" s="23"/>
-    </row>
-    <row r="43" spans="1:10" ht="22.5">
-      <c r="A43" s="18" t="s">
+      <c r="D42" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="E42"/>
+    </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B43" s="19">
+      <c r="B43" s="17">
         <v>2</v>
       </c>
-      <c r="C43" s="28"/>
-      <c r="D43" s="23"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
-      <c r="I43" s="24"/>
-      <c r="J43" s="24"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="E43"/>
+      <c r="F43" s="22"/>
+      <c r="G43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
     </row>
     <row r="44" spans="1:10" ht="67.5">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B44" s="4">
@@ -3725,14 +4253,17 @@
       <c r="C44" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="D44" s="23"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24"/>
+      <c r="D44" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="E44"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" ht="67.5">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="7" t="s">
         <v>88</v>
       </c>
       <c r="B45" s="4">
@@ -3741,13 +4272,16 @@
       <c r="C45" s="3" t="s">
         <v>371</v>
       </c>
-      <c r="D45" s="23"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
+      <c r="D45" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E45"/>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+      <c r="J45" s="22"/>
     </row>
     <row r="46" spans="1:10" ht="67.5">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="7" t="s">
         <v>65</v>
       </c>
       <c r="B46" s="4">
@@ -3756,29 +4290,35 @@
       <c r="C46" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="D46" s="23"/>
-      <c r="I46" s="24"/>
-      <c r="J46" s="24"/>
+      <c r="D46" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="E46"/>
+      <c r="I46" s="22"/>
+      <c r="J46" s="22"/>
     </row>
     <row r="47" spans="1:10" ht="67.5">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B47" s="19">
+      <c r="B47" s="17">
         <v>11</v>
       </c>
-      <c r="C47" s="28" t="s">
+      <c r="C47" s="26" t="s">
         <v>297</v>
       </c>
-      <c r="D47" s="23"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="24"/>
-      <c r="H47" s="24"/>
-      <c r="I47" s="24"/>
-      <c r="J47" s="24"/>
+      <c r="D47" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="E47"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
     </row>
     <row r="48" spans="1:10" ht="67.5">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B48" s="4">
@@ -3787,63 +4327,72 @@
       <c r="C48" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="D48" s="23"/>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24"/>
-      <c r="I48" s="24"/>
-      <c r="J48" s="24"/>
+      <c r="D48" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="E48"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="22"/>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
     </row>
     <row r="49" spans="1:10" ht="67.5">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="23" t="s">
         <v>377</v>
       </c>
-      <c r="B49" s="26">
+      <c r="B49" s="24">
         <v>0</v>
       </c>
-      <c r="C49" s="39" t="s">
+      <c r="C49" s="36" t="s">
         <v>378</v>
       </c>
-      <c r="D49" s="23"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="24"/>
-      <c r="H49" s="24"/>
-      <c r="I49" s="24"/>
-      <c r="J49" s="24"/>
+      <c r="E49"/>
+      <c r="F49" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="22"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
     </row>
     <row r="50" spans="1:10" ht="67.5">
-      <c r="A50" s="18" t="s">
+      <c r="A50" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B50" s="19">
+      <c r="B50" s="17">
         <v>9</v>
       </c>
-      <c r="C50" s="28" t="s">
+      <c r="C50" s="26" t="s">
         <v>295</v>
       </c>
-      <c r="D50" s="23"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="24"/>
-      <c r="J50" s="24"/>
+      <c r="D50" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E50"/>
+      <c r="F50" s="22"/>
+      <c r="G50" s="22"/>
+      <c r="J50" s="22"/>
     </row>
     <row r="51" spans="1:10" ht="45">
-      <c r="A51" s="14" t="s">
+      <c r="A51" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="B51" s="15">
+      <c r="B51" s="13">
         <v>1</v>
       </c>
-      <c r="C51" s="17" t="s">
+      <c r="C51" s="15" t="s">
         <v>279</v>
       </c>
-      <c r="D51" s="23"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="24"/>
-      <c r="I51" s="24"/>
-      <c r="J51" s="24"/>
+      <c r="D51" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E51"/>
+      <c r="F51" s="22"/>
+      <c r="G51" s="22"/>
+      <c r="I51" s="22"/>
+      <c r="J51" s="22"/>
     </row>
     <row r="52" spans="1:10" ht="67.5">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B52" s="4">
@@ -3852,14 +4401,17 @@
       <c r="C52" s="3" t="s">
         <v>282</v>
       </c>
-      <c r="D52" s="23"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="24"/>
-      <c r="I52" s="24"/>
-      <c r="J52" s="24"/>
+      <c r="D52" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E52"/>
+      <c r="F52" s="22"/>
+      <c r="G52" s="22"/>
+      <c r="I52" s="22"/>
+      <c r="J52" s="22"/>
     </row>
     <row r="53" spans="1:10" ht="45">
-      <c r="A53" s="9" t="s">
+      <c r="A53" s="7" t="s">
         <v>3</v>
       </c>
       <c r="B53" s="4">
@@ -3868,15 +4420,18 @@
       <c r="C53" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="D53" s="23"/>
-      <c r="F53" s="24"/>
-      <c r="G53" s="24"/>
-      <c r="H53" s="24"/>
-      <c r="I53" s="24"/>
-      <c r="J53" s="24"/>
+      <c r="D53" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="E53"/>
+      <c r="F53" s="22"/>
+      <c r="G53" s="22"/>
+      <c r="H53" s="22"/>
+      <c r="I53" s="22"/>
+      <c r="J53" s="22"/>
     </row>
     <row r="54" spans="1:10" ht="45">
-      <c r="A54" s="9" t="s">
+      <c r="A54" s="7" t="s">
         <v>57</v>
       </c>
       <c r="B54" s="4">
@@ -3885,14 +4440,17 @@
       <c r="C54" s="3" t="s">
         <v>284</v>
       </c>
-      <c r="D54" s="23"/>
-      <c r="F54" s="24"/>
-      <c r="G54" s="24"/>
-      <c r="I54" s="24"/>
-      <c r="J54" s="24"/>
+      <c r="D54" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="E54"/>
+      <c r="F54" s="22"/>
+      <c r="G54" s="22"/>
+      <c r="I54" s="22"/>
+      <c r="J54" s="22"/>
     </row>
     <row r="55" spans="1:10" ht="45">
-      <c r="A55" s="9" t="s">
+      <c r="A55" s="7" t="s">
         <v>59</v>
       </c>
       <c r="B55" s="4">
@@ -3901,15 +4459,18 @@
       <c r="C55" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="D55" s="23"/>
-      <c r="F55" s="24"/>
-      <c r="G55" s="24"/>
-      <c r="H55" s="24"/>
-      <c r="I55" s="24"/>
-      <c r="J55" s="24"/>
+      <c r="D55" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E55"/>
+      <c r="F55" s="22"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="22"/>
+      <c r="I55" s="22"/>
+      <c r="J55" s="22"/>
     </row>
     <row r="56" spans="1:10" ht="45">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="7" t="s">
         <v>116</v>
       </c>
       <c r="B56" s="4">
@@ -3918,13 +4479,16 @@
       <c r="C56" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="D56" s="23"/>
-      <c r="F56" s="24"/>
-      <c r="G56" s="24"/>
-      <c r="J56" s="24"/>
+      <c r="D56" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="E56"/>
+      <c r="F56" s="22"/>
+      <c r="G56" s="22"/>
+      <c r="J56" s="22"/>
     </row>
     <row r="57" spans="1:10" ht="45">
-      <c r="A57" s="9" t="s">
+      <c r="A57" s="7" t="s">
         <v>85</v>
       </c>
       <c r="B57" s="4">
@@ -3933,13 +4497,16 @@
       <c r="C57" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="D57" s="23"/>
-      <c r="G57" s="24"/>
-      <c r="I57" s="24"/>
-      <c r="J57" s="24"/>
+      <c r="D57" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="E57"/>
+      <c r="G57" s="22"/>
+      <c r="I57" s="22"/>
+      <c r="J57" s="22"/>
     </row>
     <row r="58" spans="1:10" ht="45">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="7" t="s">
         <v>106</v>
       </c>
       <c r="B58" s="4">
@@ -3948,12 +4515,15 @@
       <c r="C58" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="D58" s="23"/>
-      <c r="I58" s="24"/>
-      <c r="J58" s="24"/>
+      <c r="D58" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="E58"/>
+      <c r="I58" s="22"/>
+      <c r="J58" s="22"/>
     </row>
     <row r="59" spans="1:10" ht="45">
-      <c r="A59" s="9" t="s">
+      <c r="A59" s="7" t="s">
         <v>93</v>
       </c>
       <c r="B59" s="4">
@@ -3962,14 +4532,17 @@
       <c r="C59" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="D59" s="23"/>
-      <c r="F59" s="24"/>
-      <c r="H59" s="24"/>
-      <c r="I59" s="24"/>
-      <c r="J59" s="24"/>
+      <c r="D59" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="E59"/>
+      <c r="F59" s="22"/>
+      <c r="H59" s="22"/>
+      <c r="I59" s="22"/>
+      <c r="J59" s="22"/>
     </row>
     <row r="60" spans="1:10" ht="90">
-      <c r="A60" s="9" t="s">
+      <c r="A60" s="7" t="s">
         <v>96</v>
       </c>
       <c r="B60" s="4">
@@ -3978,40 +4551,51 @@
       <c r="C60" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="D60" s="23"/>
-      <c r="F60" s="24"/>
-      <c r="H60" s="24"/>
-      <c r="I60" s="24"/>
-      <c r="J60" s="24"/>
-    </row>
-    <row r="61" spans="1:10" s="23" customFormat="1" ht="90">
-      <c r="A61" s="18" t="s">
+      <c r="D60" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="E60"/>
+      <c r="F60" s="22"/>
+      <c r="H60" s="22"/>
+      <c r="I60" s="22"/>
+      <c r="J60" s="22"/>
+    </row>
+    <row r="61" spans="1:10" s="21" customFormat="1" ht="90">
+      <c r="A61" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="B61" s="19">
+      <c r="B61" s="17">
         <v>1</v>
       </c>
-      <c r="C61" s="20" t="s">
+      <c r="C61" s="18" t="s">
         <v>334</v>
       </c>
-      <c r="I61" s="24"/>
-      <c r="J61" s="24"/>
-    </row>
-    <row r="62" spans="1:10" s="23" customFormat="1" ht="90">
-      <c r="A62" s="21" t="s">
+      <c r="D61" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="E61"/>
+      <c r="I61" s="22"/>
+      <c r="J61" s="22"/>
+    </row>
+    <row r="62" spans="1:10" s="21" customFormat="1" ht="90">
+      <c r="A62" s="19" t="s">
         <v>105</v>
       </c>
       <c r="B62" s="4">
         <v>17</v>
       </c>
-      <c r="C62" s="22" t="s">
+      <c r="C62" s="20" t="s">
         <v>335</v>
       </c>
-      <c r="I62" s="24"/>
-      <c r="J62" s="24"/>
+      <c r="D62" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="E62"/>
+      <c r="I62" s="22"/>
+      <c r="J62" s="22"/>
     </row>
     <row r="63" spans="1:10" ht="90">
-      <c r="A63" s="9" t="s">
+      <c r="A63" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B63" s="4">
@@ -4020,11 +4604,14 @@
       <c r="C63" s="2" t="s">
         <v>336</v>
       </c>
-      <c r="D63" s="23"/>
-      <c r="J63" s="24"/>
+      <c r="D63" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="E63"/>
+      <c r="J63" s="22"/>
     </row>
     <row r="64" spans="1:10" ht="90">
-      <c r="A64" s="9" t="s">
+      <c r="A64" s="7" t="s">
         <v>129</v>
       </c>
       <c r="B64" s="4">
@@ -4033,95 +4620,113 @@
       <c r="C64" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="D64" s="23"/>
-      <c r="I64" s="24"/>
-      <c r="J64" s="24"/>
+      <c r="D64" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="E64"/>
+      <c r="I64" s="22"/>
+      <c r="J64" s="22"/>
     </row>
     <row r="65" spans="1:10" ht="45">
-      <c r="A65" s="18" t="s">
+      <c r="A65" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="B65" s="19">
+      <c r="B65" s="17">
         <v>1</v>
       </c>
-      <c r="C65" s="20" t="s">
+      <c r="C65" s="18" t="s">
         <v>338</v>
       </c>
-      <c r="D65" s="23"/>
-      <c r="I65" s="24"/>
-      <c r="J65" s="24"/>
-    </row>
-    <row r="66" spans="1:10" s="23" customFormat="1" ht="90">
-      <c r="A66" s="21" t="s">
+      <c r="D65" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="E65"/>
+      <c r="I65" s="22"/>
+      <c r="J65" s="22"/>
+    </row>
+    <row r="66" spans="1:10" s="21" customFormat="1" ht="90">
+      <c r="A66" s="19" t="s">
         <v>119</v>
       </c>
       <c r="B66" s="4">
         <v>6</v>
       </c>
-      <c r="C66" s="22" t="s">
+      <c r="C66" s="20" t="s">
         <v>355</v>
       </c>
-      <c r="I66" s="24"/>
-      <c r="J66" s="24"/>
-    </row>
-    <row r="67" spans="1:10" s="23" customFormat="1" ht="90">
-      <c r="A67" s="25" t="s">
+      <c r="D66" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="E66"/>
+      <c r="I66" s="22"/>
+      <c r="J66" s="22"/>
+    </row>
+    <row r="67" spans="1:10" s="21" customFormat="1" ht="90">
+      <c r="A67" s="23" t="s">
         <v>341</v>
       </c>
-      <c r="B67" s="26">
+      <c r="B67" s="24">
         <v>0</v>
       </c>
-      <c r="C67" s="27" t="s">
+      <c r="C67" s="25" t="s">
         <v>342</v>
       </c>
-      <c r="I67" s="24"/>
-      <c r="J67" s="24"/>
-    </row>
-    <row r="68" spans="1:10" s="23" customFormat="1" ht="90">
-      <c r="A68" s="25" t="s">
+      <c r="D67" s="2"/>
+      <c r="E67"/>
+      <c r="I67" s="22"/>
+      <c r="J67" s="22"/>
+    </row>
+    <row r="68" spans="1:10" s="21" customFormat="1" ht="90">
+      <c r="A68" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="B68" s="26">
+      <c r="B68" s="24">
         <v>0</v>
       </c>
-      <c r="C68" s="27" t="s">
+      <c r="C68" s="25" t="s">
         <v>345</v>
       </c>
-      <c r="I68" s="24"/>
-      <c r="J68" s="24"/>
-    </row>
-    <row r="69" spans="1:10" s="23" customFormat="1" ht="90">
-      <c r="A69" s="25" t="s">
+      <c r="D68" s="2"/>
+      <c r="E68"/>
+      <c r="I68" s="22"/>
+      <c r="J68" s="22"/>
+    </row>
+    <row r="69" spans="1:10" s="21" customFormat="1" ht="90">
+      <c r="A69" s="23" t="s">
         <v>340</v>
       </c>
-      <c r="B69" s="26">
+      <c r="B69" s="24">
         <v>0</v>
       </c>
-      <c r="C69" s="27" t="s">
+      <c r="C69" s="25" t="s">
         <v>346</v>
       </c>
-      <c r="F69" s="24"/>
-      <c r="G69" s="24"/>
-      <c r="H69" s="24"/>
-      <c r="I69" s="24"/>
-      <c r="J69" s="24"/>
-    </row>
-    <row r="70" spans="1:10" s="23" customFormat="1" ht="90">
-      <c r="A70" s="25" t="s">
+      <c r="D69" s="2"/>
+      <c r="E69"/>
+      <c r="F69" s="22"/>
+      <c r="G69" s="22"/>
+      <c r="H69" s="22"/>
+      <c r="I69" s="22"/>
+      <c r="J69" s="22"/>
+    </row>
+    <row r="70" spans="1:10" s="21" customFormat="1" ht="90">
+      <c r="A70" s="23" t="s">
         <v>344</v>
       </c>
-      <c r="B70" s="26">
+      <c r="B70" s="24">
         <v>0</v>
       </c>
-      <c r="C70" s="27" t="s">
+      <c r="C70" s="25" t="s">
         <v>347</v>
       </c>
-      <c r="H70" s="24"/>
-      <c r="I70" s="24"/>
-      <c r="J70" s="24"/>
+      <c r="D70" s="2"/>
+      <c r="E70"/>
+      <c r="H70" s="22"/>
+      <c r="I70" s="22"/>
+      <c r="J70" s="22"/>
     </row>
     <row r="71" spans="1:10" ht="67.5">
-      <c r="A71" s="9" t="s">
+      <c r="A71" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B71" s="4">
@@ -4130,15 +4735,18 @@
       <c r="C71" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="D71" s="23"/>
-      <c r="F71" s="24"/>
-      <c r="G71" s="24"/>
-      <c r="H71" s="24"/>
-      <c r="I71" s="24"/>
-      <c r="J71" s="24"/>
+      <c r="D71" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="E71"/>
+      <c r="F71" s="22"/>
+      <c r="G71" s="22"/>
+      <c r="H71" s="22"/>
+      <c r="I71" s="22"/>
+      <c r="J71" s="22"/>
     </row>
     <row r="72" spans="1:10" ht="67.5">
-      <c r="A72" s="9" t="s">
+      <c r="A72" s="7" t="s">
         <v>95</v>
       </c>
       <c r="B72" s="4">
@@ -4147,15 +4755,18 @@
       <c r="C72" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="D72" s="23"/>
-      <c r="F72" s="24"/>
-      <c r="G72" s="24"/>
-      <c r="H72" s="24"/>
-      <c r="I72" s="24"/>
-      <c r="J72" s="24"/>
+      <c r="D72" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="E72"/>
+      <c r="F72" s="22"/>
+      <c r="G72" s="22"/>
+      <c r="H72" s="22"/>
+      <c r="I72" s="22"/>
+      <c r="J72" s="22"/>
     </row>
     <row r="73" spans="1:10" ht="45">
-      <c r="A73" s="9" t="s">
+      <c r="A73" s="7" t="s">
         <v>73</v>
       </c>
       <c r="B73" s="4">
@@ -4164,15 +4775,18 @@
       <c r="C73" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="D73" s="23"/>
-      <c r="F73" s="24"/>
-      <c r="G73" s="24"/>
-      <c r="H73" s="24"/>
-      <c r="I73" s="24"/>
-      <c r="J73" s="24"/>
+      <c r="D73" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="E73"/>
+      <c r="F73" s="22"/>
+      <c r="G73" s="22"/>
+      <c r="H73" s="22"/>
+      <c r="I73" s="22"/>
+      <c r="J73" s="22"/>
     </row>
     <row r="74" spans="1:10" ht="45">
-      <c r="A74" s="9" t="s">
+      <c r="A74" s="7" t="s">
         <v>72</v>
       </c>
       <c r="B74" s="4">
@@ -4181,15 +4795,18 @@
       <c r="C74" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="D74" s="23"/>
-      <c r="F74" s="24"/>
-      <c r="G74" s="24"/>
-      <c r="H74" s="24"/>
-      <c r="I74" s="24"/>
-      <c r="J74" s="24"/>
+      <c r="D74" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="E74"/>
+      <c r="F74" s="22"/>
+      <c r="G74" s="22"/>
+      <c r="H74" s="22"/>
+      <c r="I74" s="22"/>
+      <c r="J74" s="22"/>
     </row>
     <row r="75" spans="1:10" ht="45">
-      <c r="A75" s="9" t="s">
+      <c r="A75" s="7" t="s">
         <v>69</v>
       </c>
       <c r="B75" s="4">
@@ -4198,29 +4815,35 @@
       <c r="C75" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="D75" s="23"/>
-      <c r="F75" s="24"/>
-      <c r="G75" s="24"/>
-      <c r="J75" s="24"/>
+      <c r="D75" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="E75"/>
+      <c r="F75" s="22"/>
+      <c r="G75" s="22"/>
+      <c r="J75" s="22"/>
     </row>
     <row r="76" spans="1:10" ht="45">
-      <c r="A76" s="18" t="s">
+      <c r="A76" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B76" s="19">
+      <c r="B76" s="17">
         <v>2</v>
       </c>
-      <c r="C76" s="20" t="s">
+      <c r="C76" s="18" t="s">
         <v>289</v>
       </c>
-      <c r="D76" s="23"/>
-      <c r="F76" s="24"/>
-      <c r="G76" s="24"/>
-      <c r="I76" s="24"/>
-      <c r="J76" s="24"/>
+      <c r="D76" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E76"/>
+      <c r="F76" s="22"/>
+      <c r="G76" s="22"/>
+      <c r="I76" s="22"/>
+      <c r="J76" s="22"/>
     </row>
     <row r="77" spans="1:10" ht="45">
-      <c r="A77" s="9" t="s">
+      <c r="A77" s="7" t="s">
         <v>103</v>
       </c>
       <c r="B77" s="4">
@@ -4229,10 +4852,13 @@
       <c r="C77" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="D77" s="23"/>
+      <c r="D77" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="E77"/>
     </row>
     <row r="78" spans="1:10" ht="45">
-      <c r="A78" s="9" t="s">
+      <c r="A78" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B78" s="4">
@@ -4241,10 +4867,13 @@
       <c r="C78" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="D78" s="23"/>
-    </row>
-    <row r="79" spans="1:10" ht="22.5">
-      <c r="A79" s="9" t="s">
+      <c r="D78" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="E78"/>
+    </row>
+    <row r="79" spans="1:10" ht="45">
+      <c r="A79" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B79" s="4">
@@ -4253,10 +4882,13 @@
       <c r="C79" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D79" s="23"/>
+      <c r="D79" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="E79"/>
     </row>
     <row r="80" spans="1:10" ht="67.5">
-      <c r="A80" s="9" t="s">
+      <c r="A80" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B80" s="4">
@@ -4265,10 +4897,13 @@
       <c r="C80" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="D80" s="23"/>
-    </row>
-    <row r="81" spans="1:4" ht="67.5">
-      <c r="A81" s="9" t="s">
+      <c r="D80" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="E80"/>
+    </row>
+    <row r="81" spans="1:5" ht="67.5">
+      <c r="A81" s="7" t="s">
         <v>145</v>
       </c>
       <c r="B81" s="4">
@@ -4277,10 +4912,13 @@
       <c r="C81" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="D81" s="23"/>
-    </row>
-    <row r="82" spans="1:4" ht="45">
-      <c r="A82" s="9" t="s">
+      <c r="D81" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="E81"/>
+    </row>
+    <row r="82" spans="1:5" ht="45">
+      <c r="A82" s="7" t="s">
         <v>60</v>
       </c>
       <c r="B82" s="4">
@@ -4289,10 +4927,13 @@
       <c r="C82" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="D82" s="23"/>
-    </row>
-    <row r="83" spans="1:4" ht="45">
-      <c r="A83" s="9" t="s">
+      <c r="D82" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="E82"/>
+    </row>
+    <row r="83" spans="1:5" ht="45">
+      <c r="A83" s="7" t="s">
         <v>146</v>
       </c>
       <c r="B83" s="4">
@@ -4301,10 +4942,13 @@
       <c r="C83" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="D83" s="23"/>
-    </row>
-    <row r="84" spans="1:4" ht="22.5">
-      <c r="A84" s="9" t="s">
+      <c r="D83" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="E83"/>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="7" t="s">
         <v>136</v>
       </c>
       <c r="B84" s="4">
@@ -4313,10 +4957,13 @@
       <c r="C84" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="D84" s="23"/>
-    </row>
-    <row r="85" spans="1:4" ht="45">
-      <c r="A85" s="9" t="s">
+      <c r="D84" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="E84"/>
+    </row>
+    <row r="85" spans="1:5" ht="45">
+      <c r="A85" s="7" t="s">
         <v>98</v>
       </c>
       <c r="B85" s="4">
@@ -4325,10 +4972,13 @@
       <c r="C85" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="D85" s="23"/>
-    </row>
-    <row r="86" spans="1:4" ht="45">
-      <c r="A86" s="9" t="s">
+      <c r="D85" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="E85"/>
+    </row>
+    <row r="86" spans="1:5" ht="45">
+      <c r="A86" s="7" t="s">
         <v>99</v>
       </c>
       <c r="B86" s="4">
@@ -4337,10 +4987,13 @@
       <c r="C86" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="D86" s="23"/>
-    </row>
-    <row r="87" spans="1:4" ht="22.5">
-      <c r="A87" s="9" t="s">
+      <c r="D86" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="E86"/>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B87" s="4">
@@ -4349,10 +5002,13 @@
       <c r="C87" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="D87" s="23"/>
-    </row>
-    <row r="88" spans="1:4" ht="22.5">
-      <c r="A88" s="9" t="s">
+      <c r="D87" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="E87"/>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="7" t="s">
         <v>118</v>
       </c>
       <c r="B88" s="4">
@@ -4361,10 +5017,13 @@
       <c r="C88" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="D88" s="23"/>
-    </row>
-    <row r="89" spans="1:4" ht="22.5">
-      <c r="A89" s="9" t="s">
+      <c r="D88" s="2" t="s">
+        <v>448</v>
+      </c>
+      <c r="E88"/>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B89" s="4">
@@ -4373,10 +5032,13 @@
       <c r="C89" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="D89" s="23"/>
-    </row>
-    <row r="90" spans="1:4" ht="22.5">
-      <c r="A90" s="9" t="s">
+      <c r="D89" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="E89"/>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="7" t="s">
         <v>138</v>
       </c>
       <c r="B90" s="4">
@@ -4385,10 +5047,13 @@
       <c r="C90" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D90" s="23"/>
-    </row>
-    <row r="91" spans="1:4" ht="22.5">
-      <c r="A91" s="9" t="s">
+      <c r="D90" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="E90"/>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="7" t="s">
         <v>112</v>
       </c>
       <c r="B91" s="4">
@@ -4397,10 +5062,13 @@
       <c r="C91" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="D91" s="23"/>
-    </row>
-    <row r="92" spans="1:4" ht="90">
-      <c r="A92" s="9" t="s">
+      <c r="D91" s="2" t="s">
+        <v>451</v>
+      </c>
+      <c r="E91"/>
+    </row>
+    <row r="92" spans="1:5" ht="90">
+      <c r="A92" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B92" s="4">
@@ -4409,10 +5077,13 @@
       <c r="C92" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D92" s="23"/>
-    </row>
-    <row r="93" spans="1:4" ht="90">
-      <c r="A93" s="9" t="s">
+      <c r="D92" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="E92"/>
+    </row>
+    <row r="93" spans="1:5" ht="90">
+      <c r="A93" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B93" s="4">
@@ -4421,10 +5092,13 @@
       <c r="C93" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="D93" s="23"/>
-    </row>
-    <row r="94" spans="1:4" ht="45">
-      <c r="A94" s="9" t="s">
+      <c r="D93" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="E93"/>
+    </row>
+    <row r="94" spans="1:5" ht="45">
+      <c r="A94" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B94" s="4">
@@ -4433,10 +5107,13 @@
       <c r="C94" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="D94" s="23"/>
-    </row>
-    <row r="95" spans="1:4" ht="45">
-      <c r="A95" s="9" t="s">
+      <c r="D94" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="E94"/>
+    </row>
+    <row r="95" spans="1:5" ht="45">
+      <c r="A95" s="7" t="s">
         <v>135</v>
       </c>
       <c r="B95" s="4">
@@ -4445,10 +5122,13 @@
       <c r="C95" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="D95" s="23"/>
-    </row>
-    <row r="96" spans="1:4" ht="67.5">
-      <c r="A96" s="9" t="s">
+      <c r="D95" s="2" t="s">
+        <v>455</v>
+      </c>
+      <c r="E95"/>
+    </row>
+    <row r="96" spans="1:5" ht="67.5">
+      <c r="A96" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B96" s="4">
@@ -4457,10 +5137,13 @@
       <c r="C96" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D96" s="23"/>
-    </row>
-    <row r="97" spans="1:4" ht="67.5">
-      <c r="A97" s="9" t="s">
+      <c r="D96" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="E96"/>
+    </row>
+    <row r="97" spans="1:5" ht="67.5">
+      <c r="A97" s="7" t="s">
         <v>141</v>
       </c>
       <c r="B97" s="4">
@@ -4469,10 +5152,13 @@
       <c r="C97" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D97" s="23"/>
-    </row>
-    <row r="98" spans="1:4" ht="67.5">
-      <c r="A98" s="9" t="s">
+      <c r="D97" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="E97"/>
+    </row>
+    <row r="98" spans="1:5" ht="67.5">
+      <c r="A98" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B98" s="4">
@@ -4481,10 +5167,13 @@
       <c r="C98" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="D98" s="23"/>
-    </row>
-    <row r="99" spans="1:4" ht="67.5">
-      <c r="A99" s="9" t="s">
+      <c r="D98" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="E98"/>
+    </row>
+    <row r="99" spans="1:5" ht="67.5">
+      <c r="A99" s="7" t="s">
         <v>19</v>
       </c>
       <c r="B99" s="4">
@@ -4493,10 +5182,13 @@
       <c r="C99" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D99" s="23"/>
-    </row>
-    <row r="100" spans="1:4" ht="67.5">
-      <c r="A100" s="9" t="s">
+      <c r="D99" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="E99"/>
+    </row>
+    <row r="100" spans="1:5" ht="67.5">
+      <c r="A100" s="7" t="s">
         <v>134</v>
       </c>
       <c r="B100" s="4">
@@ -4505,10 +5197,13 @@
       <c r="C100" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="D100" s="23"/>
-    </row>
-    <row r="101" spans="1:4" ht="67.5">
-      <c r="A101" s="9" t="s">
+      <c r="D100" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="E100"/>
+    </row>
+    <row r="101" spans="1:5" ht="67.5">
+      <c r="A101" s="7" t="s">
         <v>137</v>
       </c>
       <c r="B101" s="4">
@@ -4517,10 +5212,13 @@
       <c r="C101" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="D101" s="23"/>
-    </row>
-    <row r="102" spans="1:4" ht="67.5">
-      <c r="A102" s="9" t="s">
+      <c r="D101" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="E101"/>
+    </row>
+    <row r="102" spans="1:5" ht="67.5">
+      <c r="A102" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B102" s="4">
@@ -4529,10 +5227,13 @@
       <c r="C102" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D102" s="23"/>
-    </row>
-    <row r="103" spans="1:4" ht="67.5">
-      <c r="A103" s="9" t="s">
+      <c r="D102" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="E102"/>
+    </row>
+    <row r="103" spans="1:5" ht="67.5">
+      <c r="A103" s="7" t="s">
         <v>147</v>
       </c>
       <c r="B103" s="4">
@@ -4541,10 +5242,13 @@
       <c r="C103" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="D103" s="23"/>
-    </row>
-    <row r="104" spans="1:4" ht="90">
-      <c r="A104" s="9" t="s">
+      <c r="D103" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="E103"/>
+    </row>
+    <row r="104" spans="1:5" ht="90">
+      <c r="A104" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B104" s="4">
@@ -4553,10 +5257,13 @@
       <c r="C104" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="D104" s="23"/>
-    </row>
-    <row r="105" spans="1:4" ht="90">
-      <c r="A105" s="9" t="s">
+      <c r="D104" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="E104"/>
+    </row>
+    <row r="105" spans="1:5" ht="90">
+      <c r="A105" s="7" t="s">
         <v>142</v>
       </c>
       <c r="B105" s="4">
@@ -4565,10 +5272,13 @@
       <c r="C105" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="D105" s="23"/>
-    </row>
-    <row r="106" spans="1:4" ht="45">
-      <c r="A106" s="9" t="s">
+      <c r="D105" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="E105"/>
+    </row>
+    <row r="106" spans="1:5" ht="45">
+      <c r="A106" s="7" t="s">
         <v>42</v>
       </c>
       <c r="B106" s="4">
@@ -4577,10 +5287,13 @@
       <c r="C106" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="D106" s="23"/>
-    </row>
-    <row r="107" spans="1:4" ht="45">
-      <c r="A107" s="9" t="s">
+      <c r="D106" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="E106"/>
+    </row>
+    <row r="107" spans="1:5" ht="45">
+      <c r="A107" s="7" t="s">
         <v>148</v>
       </c>
       <c r="B107" s="4">
@@ -4589,10 +5302,13 @@
       <c r="C107" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="D107" s="23"/>
-    </row>
-    <row r="108" spans="1:4" ht="22.5">
-      <c r="A108" s="9" t="s">
+      <c r="D107" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="E107"/>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="7" t="s">
         <v>76</v>
       </c>
       <c r="B108" s="4">
@@ -4601,10 +5317,13 @@
       <c r="C108" s="2" t="s">
         <v>331</v>
       </c>
-      <c r="D108" s="23"/>
-    </row>
-    <row r="109" spans="1:4" ht="22.5">
-      <c r="A109" s="9" t="s">
+      <c r="D108" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E108"/>
+    </row>
+    <row r="109" spans="1:5" ht="45">
+      <c r="A109" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B109" s="4">
@@ -4613,10 +5332,13 @@
       <c r="C109" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D109" s="23"/>
-    </row>
-    <row r="110" spans="1:4" ht="22.5">
-      <c r="A110" s="9" t="s">
+      <c r="D109" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="E109"/>
+    </row>
+    <row r="110" spans="1:5">
+      <c r="A110" s="7" t="s">
         <v>143</v>
       </c>
       <c r="B110" s="4">
@@ -4625,10 +5347,13 @@
       <c r="C110" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D110" s="23"/>
-    </row>
-    <row r="111" spans="1:4" ht="45">
-      <c r="A111" s="9" t="s">
+      <c r="D110" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="E110"/>
+    </row>
+    <row r="111" spans="1:5" ht="45">
+      <c r="A111" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B111" s="4">
@@ -4637,10 +5362,13 @@
       <c r="C111" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="D111" s="23"/>
-    </row>
-    <row r="112" spans="1:4" ht="45">
-      <c r="A112" s="9" t="s">
+      <c r="D111" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="E111"/>
+    </row>
+    <row r="112" spans="1:5" ht="45">
+      <c r="A112" s="7" t="s">
         <v>149</v>
       </c>
       <c r="B112" s="4">
@@ -4649,10 +5377,13 @@
       <c r="C112" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="D112" s="23"/>
-    </row>
-    <row r="113" spans="1:4" ht="45">
-      <c r="A113" s="9" t="s">
+      <c r="D112" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="E112"/>
+    </row>
+    <row r="113" spans="1:5" ht="45">
+      <c r="A113" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B113" s="4">
@@ -4661,10 +5392,13 @@
       <c r="C113" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D113" s="23"/>
-    </row>
-    <row r="114" spans="1:4" ht="45">
-      <c r="A114" s="9" t="s">
+      <c r="D113" s="2" t="s">
+        <v>473</v>
+      </c>
+      <c r="E113"/>
+    </row>
+    <row r="114" spans="1:5" ht="45">
+      <c r="A114" s="7" t="s">
         <v>144</v>
       </c>
       <c r="B114" s="4">
@@ -4673,10 +5407,13 @@
       <c r="C114" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D114" s="23"/>
-    </row>
-    <row r="115" spans="1:4" ht="22.5">
-      <c r="A115" s="9" t="s">
+      <c r="D114" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="E114"/>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" s="7" t="s">
         <v>68</v>
       </c>
       <c r="B115" s="4">
@@ -4685,10 +5422,13 @@
       <c r="C115" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="D115" s="23"/>
-    </row>
-    <row r="116" spans="1:4" ht="67.5">
-      <c r="A116" s="9" t="s">
+      <c r="D115" s="2" t="s">
+        <v>475</v>
+      </c>
+      <c r="E115"/>
+    </row>
+    <row r="116" spans="1:5" ht="67.5">
+      <c r="A116" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B116" s="4">
@@ -4697,10 +5437,13 @@
       <c r="C116" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="D116" s="23"/>
-    </row>
-    <row r="117" spans="1:4" ht="67.5">
-      <c r="A117" s="9" t="s">
+      <c r="D116" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="E116"/>
+    </row>
+    <row r="117" spans="1:5" ht="67.5">
+      <c r="A117" s="7" t="s">
         <v>102</v>
       </c>
       <c r="B117" s="4">
@@ -4709,10 +5452,13 @@
       <c r="C117" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="D117" s="23"/>
-    </row>
-    <row r="118" spans="1:4" ht="45">
-      <c r="A118" s="9" t="s">
+      <c r="D117" s="2" t="s">
+        <v>477</v>
+      </c>
+      <c r="E117"/>
+    </row>
+    <row r="118" spans="1:5" ht="45">
+      <c r="A118" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B118" s="4">
@@ -4721,10 +5467,13 @@
       <c r="C118" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="D118" s="23"/>
-    </row>
-    <row r="119" spans="1:4" ht="45">
-      <c r="A119" s="9" t="s">
+      <c r="D118" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="E118"/>
+    </row>
+    <row r="119" spans="1:5" ht="45">
+      <c r="A119" s="7" t="s">
         <v>139</v>
       </c>
       <c r="B119" s="4">
@@ -4733,10 +5482,13 @@
       <c r="C119" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D119" s="23"/>
-    </row>
-    <row r="120" spans="1:4" ht="45">
-      <c r="A120" s="9" t="s">
+      <c r="D119" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="E119"/>
+    </row>
+    <row r="120" spans="1:5" ht="45">
+      <c r="A120" s="7" t="s">
         <v>123</v>
       </c>
       <c r="B120" s="4">
@@ -4745,10 +5497,13 @@
       <c r="C120" s="2" t="s">
         <v>333</v>
       </c>
-      <c r="D120" s="23"/>
-    </row>
-    <row r="121" spans="1:4" ht="45">
-      <c r="A121" s="9" t="s">
+      <c r="D120" s="2" t="s">
+        <v>480</v>
+      </c>
+      <c r="E120"/>
+    </row>
+    <row r="121" spans="1:5" ht="45">
+      <c r="A121" s="7" t="s">
         <v>122</v>
       </c>
       <c r="B121" s="4">
@@ -4757,10 +5512,13 @@
       <c r="C121" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D121" s="23"/>
-    </row>
-    <row r="122" spans="1:4" ht="67.5">
-      <c r="A122" s="9" t="s">
+      <c r="D121" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="E121"/>
+    </row>
+    <row r="122" spans="1:5" ht="67.5">
+      <c r="A122" s="7" t="s">
         <v>28</v>
       </c>
       <c r="B122" s="4">
@@ -4769,10 +5527,13 @@
       <c r="C122" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D122" s="23"/>
-    </row>
-    <row r="123" spans="1:4" ht="67.5">
-      <c r="A123" s="9" t="s">
+      <c r="D122" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="E122"/>
+    </row>
+    <row r="123" spans="1:5" ht="67.5">
+      <c r="A123" s="7" t="s">
         <v>140</v>
       </c>
       <c r="B123" s="4">
@@ -4781,10 +5542,13 @@
       <c r="C123" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="D123" s="23"/>
-    </row>
-    <row r="124" spans="1:4" ht="22.5">
-      <c r="A124" s="9" t="s">
+      <c r="D123" s="2" t="s">
+        <v>483</v>
+      </c>
+      <c r="E123"/>
+    </row>
+    <row r="124" spans="1:5">
+      <c r="A124" s="7" t="s">
         <v>53</v>
       </c>
       <c r="B124" s="4">
@@ -4793,10 +5557,13 @@
       <c r="C124" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="D124" s="23"/>
-    </row>
-    <row r="125" spans="1:4" ht="22.5">
-      <c r="A125" s="9" t="s">
+      <c r="D124" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="E124"/>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B125" s="4">
@@ -4805,10 +5572,13 @@
       <c r="C125" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="D125" s="23"/>
-    </row>
-    <row r="126" spans="1:4" ht="22.5">
-      <c r="A126" s="9" t="s">
+      <c r="D125" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="E125"/>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" s="7" t="s">
         <v>111</v>
       </c>
       <c r="B126" s="4">
@@ -4817,10 +5587,13 @@
       <c r="C126" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D126" s="23"/>
-    </row>
-    <row r="127" spans="1:4" ht="34.5">
-      <c r="A127" s="9" t="s">
+      <c r="D126" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="E126"/>
+    </row>
+    <row r="127" spans="1:5" ht="34.5">
+      <c r="A127" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B127" s="4">
@@ -4829,10 +5602,13 @@
       <c r="C127" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D127" s="23"/>
-    </row>
-    <row r="128" spans="1:4" ht="34.5">
-      <c r="A128" s="9" t="s">
+      <c r="D127" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="E127"/>
+    </row>
+    <row r="128" spans="1:5" ht="34.5">
+      <c r="A128" s="7" t="s">
         <v>151</v>
       </c>
       <c r="B128" s="4">
@@ -4841,10 +5617,13 @@
       <c r="C128" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="D128" s="23"/>
-    </row>
-    <row r="129" spans="1:4" ht="22.5">
-      <c r="A129" s="9" t="s">
+      <c r="D128" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="E128"/>
+    </row>
+    <row r="129" spans="1:5" ht="45">
+      <c r="A129" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B129" s="4">
@@ -4853,10 +5632,13 @@
       <c r="C129" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D129" s="23"/>
-    </row>
-    <row r="130" spans="1:4" ht="22.5">
-      <c r="A130" s="9" t="s">
+      <c r="D129" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="E129"/>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" s="7" t="s">
         <v>30</v>
       </c>
       <c r="B130" s="4">
@@ -4865,10 +5647,13 @@
       <c r="C130" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D130" s="23"/>
-    </row>
-    <row r="131" spans="1:4" ht="22.5">
-      <c r="A131" s="9" t="s">
+      <c r="D130" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="E130"/>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" s="7" t="s">
         <v>79</v>
       </c>
       <c r="B131" s="4">
@@ -4877,10 +5662,13 @@
       <c r="C131" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D131" s="23"/>
-    </row>
-    <row r="132" spans="1:4" ht="45">
-      <c r="A132" s="9" t="s">
+      <c r="D131" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="E131"/>
+    </row>
+    <row r="132" spans="1:5" ht="45">
+      <c r="A132" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B132" s="4">
@@ -4889,46 +5677,58 @@
       <c r="C132" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D132" s="23"/>
-    </row>
-    <row r="133" spans="1:4" ht="67.5">
-      <c r="A133" s="9" t="s">
+      <c r="D132" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="E132"/>
+    </row>
+    <row r="133" spans="1:5" ht="67.5">
+      <c r="A133" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B133" s="4">
         <v>1183</v>
       </c>
-      <c r="C133" s="10" t="s">
+      <c r="C133" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="D133" s="23"/>
-    </row>
-    <row r="134" spans="1:4" ht="67.5">
-      <c r="A134" s="9" t="s">
+      <c r="D133" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="E133"/>
+    </row>
+    <row r="134" spans="1:5" ht="67.5">
+      <c r="A134" s="7" t="s">
         <v>56</v>
       </c>
       <c r="B134" s="4">
         <v>326</v>
       </c>
-      <c r="C134" s="10" t="s">
+      <c r="C134" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="D134" s="23"/>
-    </row>
-    <row r="135" spans="1:4" ht="67.5">
-      <c r="A135" s="9" t="s">
+      <c r="D134" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="E134"/>
+    </row>
+    <row r="135" spans="1:5" ht="67.5">
+      <c r="A135" s="7" t="s">
         <v>121</v>
       </c>
       <c r="B135" s="4">
         <v>3</v>
       </c>
-      <c r="C135" s="10" t="s">
+      <c r="C135" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="D135" s="23"/>
-    </row>
-    <row r="136" spans="1:4" ht="45">
-      <c r="A136" s="9" t="s">
+      <c r="D135" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="E135"/>
+    </row>
+    <row r="136" spans="1:5" ht="45">
+      <c r="A136" s="7" t="s">
         <v>110</v>
       </c>
       <c r="B136" s="4">
@@ -4937,10 +5737,13 @@
       <c r="C136" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D136" s="23"/>
-    </row>
-    <row r="137" spans="1:4" ht="45">
-      <c r="A137" s="9" t="s">
+      <c r="D136" s="2" t="s">
+        <v>496</v>
+      </c>
+      <c r="E136"/>
+    </row>
+    <row r="137" spans="1:5" ht="45">
+      <c r="A137" s="7" t="s">
         <v>109</v>
       </c>
       <c r="B137" s="4">
@@ -4949,10 +5752,13 @@
       <c r="C137" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="D137" s="23"/>
-    </row>
-    <row r="138" spans="1:4" ht="22.5">
-      <c r="A138" s="9" t="s">
+      <c r="D137" s="2" t="s">
+        <v>497</v>
+      </c>
+      <c r="E137"/>
+    </row>
+    <row r="138" spans="1:5">
+      <c r="A138" s="7" t="s">
         <v>91</v>
       </c>
       <c r="B138" s="4">
@@ -4961,10 +5767,13 @@
       <c r="C138" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="D138" s="23"/>
-    </row>
-    <row r="139" spans="1:4" ht="34.5">
-      <c r="A139" s="9" t="s">
+      <c r="D138" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="E138"/>
+    </row>
+    <row r="139" spans="1:5" ht="34.5">
+      <c r="A139" s="7" t="s">
         <v>92</v>
       </c>
       <c r="B139" s="4">
@@ -4973,10 +5782,13 @@
       <c r="C139" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="D139" s="23"/>
-    </row>
-    <row r="140" spans="1:4" ht="45">
-      <c r="A140" s="9" t="s">
+      <c r="D139" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="E139"/>
+    </row>
+    <row r="140" spans="1:5" ht="45">
+      <c r="A140" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B140" s="4">
@@ -4985,10 +5797,13 @@
       <c r="C140" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D140" s="23"/>
-    </row>
-    <row r="141" spans="1:4" ht="22.5">
-      <c r="A141" s="9" t="s">
+      <c r="D140" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="E140"/>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B141" s="4">
@@ -4997,46 +5812,58 @@
       <c r="C141" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="D141" s="23"/>
-    </row>
-    <row r="142" spans="1:4" ht="45">
-      <c r="A142" s="9" t="s">
+      <c r="D141" s="2" t="s">
+        <v>501</v>
+      </c>
+      <c r="E141"/>
+    </row>
+    <row r="142" spans="1:5" ht="45">
+      <c r="A142" s="7" t="s">
         <v>74</v>
       </c>
       <c r="B142" s="4">
         <v>40</v>
       </c>
-      <c r="C142" s="10" t="s">
+      <c r="C142" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="D142" s="23"/>
-    </row>
-    <row r="143" spans="1:4" ht="34.5">
-      <c r="A143" s="9" t="s">
+      <c r="D142" s="2" t="s">
+        <v>502</v>
+      </c>
+      <c r="E142"/>
+    </row>
+    <row r="143" spans="1:5" ht="34.5">
+      <c r="A143" s="7" t="s">
         <v>80</v>
       </c>
       <c r="B143" s="4">
         <v>46</v>
       </c>
-      <c r="C143" s="10" t="s">
+      <c r="C143" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="D143" s="23"/>
-    </row>
-    <row r="144" spans="1:4" ht="45">
-      <c r="A144" s="9" t="s">
+      <c r="D143" s="2" t="s">
+        <v>503</v>
+      </c>
+      <c r="E143"/>
+    </row>
+    <row r="144" spans="1:5" ht="45">
+      <c r="A144" s="7" t="s">
         <v>113</v>
       </c>
       <c r="B144" s="4">
         <v>2</v>
       </c>
-      <c r="C144" s="10" t="s">
+      <c r="C144" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="D144" s="23"/>
-    </row>
-    <row r="145" spans="1:4" ht="22.5">
-      <c r="A145" s="9" t="s">
+      <c r="D144" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="E144"/>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="A145" s="7" t="s">
         <v>67</v>
       </c>
       <c r="B145" s="4">
@@ -5045,10 +5872,13 @@
       <c r="C145" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="D145" s="23"/>
-    </row>
-    <row r="146" spans="1:4" ht="45">
-      <c r="A146" s="9" t="s">
+      <c r="D145" s="2" t="s">
+        <v>505</v>
+      </c>
+      <c r="E145"/>
+    </row>
+    <row r="146" spans="1:5" ht="45">
+      <c r="A146" s="7" t="s">
         <v>120</v>
       </c>
       <c r="B146" s="4">
@@ -5057,10 +5887,13 @@
       <c r="C146" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="D146" s="23"/>
-    </row>
-    <row r="147" spans="1:4" ht="67.5">
-      <c r="A147" s="9" t="s">
+      <c r="D146" s="2" t="s">
+        <v>506</v>
+      </c>
+      <c r="E146"/>
+    </row>
+    <row r="147" spans="1:5" ht="67.5">
+      <c r="A147" s="7" t="s">
         <v>114</v>
       </c>
       <c r="B147" s="4">
@@ -5069,10 +5902,13 @@
       <c r="C147" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="D147" s="23"/>
-    </row>
-    <row r="148" spans="1:4" ht="22.5">
-      <c r="A148" s="9" t="s">
+      <c r="D147" s="2" t="s">
+        <v>507</v>
+      </c>
+      <c r="E147"/>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="A148" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B148" s="4">
@@ -5081,10 +5917,13 @@
       <c r="C148" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D148" s="23"/>
-    </row>
-    <row r="149" spans="1:4" ht="34.5">
-      <c r="A149" s="9" t="s">
+      <c r="D148" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="E148"/>
+    </row>
+    <row r="149" spans="1:5" ht="34.5">
+      <c r="A149" s="7" t="s">
         <v>51</v>
       </c>
       <c r="B149" s="4">
@@ -5093,10 +5932,13 @@
       <c r="C149" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D149" s="23"/>
-    </row>
-    <row r="150" spans="1:4" ht="45">
-      <c r="A150" s="9" t="s">
+      <c r="D149" s="2" t="s">
+        <v>509</v>
+      </c>
+      <c r="E149"/>
+    </row>
+    <row r="150" spans="1:5" ht="45">
+      <c r="A150" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B150" s="4">
@@ -5105,10 +5947,13 @@
       <c r="C150" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="D150" s="23"/>
-    </row>
-    <row r="151" spans="1:4" ht="45">
-      <c r="A151" s="9" t="s">
+      <c r="D150" s="2" t="s">
+        <v>510</v>
+      </c>
+      <c r="E150"/>
+    </row>
+    <row r="151" spans="1:5" ht="45">
+      <c r="A151" s="7" t="s">
         <v>55</v>
       </c>
       <c r="B151" s="4">
@@ -5117,10 +5962,13 @@
       <c r="C151" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="D151" s="23"/>
-    </row>
-    <row r="152" spans="1:4" ht="67.5">
-      <c r="A152" s="9" t="s">
+      <c r="D151" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="E151"/>
+    </row>
+    <row r="152" spans="1:5" ht="67.5">
+      <c r="A152" s="7" t="s">
         <v>108</v>
       </c>
       <c r="B152" s="4">
@@ -5129,10 +5977,13 @@
       <c r="C152" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="D152" s="23"/>
-    </row>
-    <row r="153" spans="1:4" ht="67.5">
-      <c r="A153" s="9" t="s">
+      <c r="D152" s="2" t="s">
+        <v>512</v>
+      </c>
+      <c r="E152"/>
+    </row>
+    <row r="153" spans="1:5" ht="67.5">
+      <c r="A153" s="7" t="s">
         <v>130</v>
       </c>
       <c r="B153" s="4">
@@ -5141,10 +5992,13 @@
       <c r="C153" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="D153" s="23"/>
-    </row>
-    <row r="154" spans="1:4" ht="45">
-      <c r="A154" s="9" t="s">
+      <c r="D153" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="E153"/>
+    </row>
+    <row r="154" spans="1:5" ht="45">
+      <c r="A154" s="7" t="s">
         <v>75</v>
       </c>
       <c r="B154" s="4">
@@ -5153,10 +6007,13 @@
       <c r="C154" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D154" s="23"/>
-    </row>
-    <row r="155" spans="1:4" ht="45">
-      <c r="A155" s="9" t="s">
+      <c r="D154" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="E154"/>
+    </row>
+    <row r="155" spans="1:5" ht="45">
+      <c r="A155" s="7" t="s">
         <v>81</v>
       </c>
       <c r="B155" s="4">
@@ -5165,10 +6022,13 @@
       <c r="C155" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D155" s="23"/>
-    </row>
-    <row r="156" spans="1:4" ht="45">
-      <c r="A156" s="9" t="s">
+      <c r="D155" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="E155"/>
+    </row>
+    <row r="156" spans="1:5" ht="45">
+      <c r="A156" s="7" t="s">
         <v>156</v>
       </c>
       <c r="B156" s="4">
@@ -5177,10 +6037,13 @@
       <c r="C156" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D156" s="23"/>
-    </row>
-    <row r="157" spans="1:4" ht="45">
-      <c r="A157" s="9" t="s">
+      <c r="D156" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="E156"/>
+    </row>
+    <row r="157" spans="1:5" ht="45">
+      <c r="A157" s="7" t="s">
         <v>90</v>
       </c>
       <c r="B157" s="4">
@@ -5189,10 +6052,13 @@
       <c r="C157" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D157" s="23"/>
-    </row>
-    <row r="158" spans="1:4" ht="22.5">
-      <c r="A158" s="9" t="s">
+      <c r="D157" s="2" t="s">
+        <v>517</v>
+      </c>
+      <c r="E157"/>
+    </row>
+    <row r="158" spans="1:5">
+      <c r="A158" s="7" t="s">
         <v>101</v>
       </c>
       <c r="B158" s="4">
@@ -5201,10 +6067,13 @@
       <c r="C158" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="D158" s="23"/>
-    </row>
-    <row r="159" spans="1:4" ht="22.5">
-      <c r="A159" s="9" t="s">
+      <c r="D158" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="E158"/>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="A159" s="7" t="s">
         <v>89</v>
       </c>
       <c r="B159" s="4">
@@ -5213,10 +6082,13 @@
       <c r="C159" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D159" s="23"/>
-    </row>
-    <row r="160" spans="1:4" ht="22.5">
-      <c r="A160" s="9" t="s">
+      <c r="D159" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="E159"/>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="A160" s="7" t="s">
         <v>100</v>
       </c>
       <c r="B160" s="4">
@@ -5225,10 +6097,13 @@
       <c r="C160" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D160" s="23"/>
-    </row>
-    <row r="161" spans="1:4" ht="22.5">
-      <c r="A161" s="9" t="s">
+      <c r="D160" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="E160"/>
+    </row>
+    <row r="161" spans="1:5">
+      <c r="A161" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B161" s="4">
@@ -5237,10 +6112,13 @@
       <c r="C161" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D161" s="23"/>
-    </row>
-    <row r="162" spans="1:4" ht="22.5">
-      <c r="A162" s="9" t="s">
+      <c r="D161" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="E161"/>
+    </row>
+    <row r="162" spans="1:5">
+      <c r="A162" s="7" t="s">
         <v>71</v>
       </c>
       <c r="B162" s="4">
@@ -5249,10 +6127,13 @@
       <c r="C162" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="D162" s="23"/>
-    </row>
-    <row r="163" spans="1:4" ht="45">
-      <c r="A163" s="9" t="s">
+      <c r="D162" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="E162"/>
+    </row>
+    <row r="163" spans="1:5" ht="45">
+      <c r="A163" s="7" t="s">
         <v>131</v>
       </c>
       <c r="B163" s="4">
@@ -5261,10 +6142,13 @@
       <c r="C163" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="D163" s="23"/>
-    </row>
-    <row r="164" spans="1:4" ht="22.5">
-      <c r="A164" s="9" t="s">
+      <c r="D163" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="E163"/>
+    </row>
+    <row r="164" spans="1:5">
+      <c r="A164" s="7" t="s">
         <v>83</v>
       </c>
       <c r="B164" s="4">
@@ -5273,9 +6157,13 @@
       <c r="C164" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" ht="22.5">
-      <c r="A165" s="9" t="s">
+      <c r="D164" s="2" t="s">
+        <v>524</v>
+      </c>
+      <c r="E164"/>
+    </row>
+    <row r="165" spans="1:5">
+      <c r="A165" s="7" t="s">
         <v>104</v>
       </c>
       <c r="B165" s="4">
@@ -5284,9 +6172,13 @@
       <c r="C165" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="166" spans="1:4">
-      <c r="A166" s="11"/>
+      <c r="D165" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="E165"/>
+    </row>
+    <row r="166" spans="1:5">
+      <c r="A166" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5409,7 +6301,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5"/>
   <cols>
-    <col min="1" max="1" width="119.5703125" style="22" customWidth="1"/>
+    <col min="1" max="1" width="119.5703125" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5418,7 +6310,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="30" t="s">
         <v>198</v>
       </c>
       <c r="B3" t="s">
@@ -5426,7 +6318,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="31" t="s">
         <v>194</v>
       </c>
       <c r="B4" t="s">
@@ -5434,132 +6326,132 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="35" t="s">
+      <c r="A5" s="32" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="32" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="32" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="20" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="20" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="32" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="32" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="20" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="14" spans="1:2">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="33" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="45">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="33" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="20" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="32" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="32" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="20" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="20" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="20" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="33" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="20" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="45">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="20" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="20" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="20" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="34" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="20" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="67.5">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="20" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="20" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="35" t="s">
+      <c r="A31" s="32" t="s">
         <v>369</v>
       </c>
     </row>
@@ -5580,71 +6472,71 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="99.85546875" style="12" customWidth="1"/>
+    <col min="1" max="1" width="99.85546875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="27" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="45">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="28" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="29" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="10" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="10" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="10" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="30">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="27" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="10" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="45">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="27" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="45">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="10" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="10" t="s">
         <v>376</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added rules for Perfect Verbs (PV tags). option yet to be programmed,
</commit_message>
<xml_diff>
--- a/TagsComments.xlsx
+++ b/TagsComments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="360" windowWidth="7980" windowHeight="5205" activeTab="1"/>
+    <workbookView xWindow="720" yWindow="360" windowWidth="7980" windowHeight="5205" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Count" sheetId="9" r:id="rId1"/>
@@ -49,6 +49,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Examples are copied from dictStems verbatim.</t>
         </r>
@@ -220,12 +221,87 @@
         </r>
       </text>
     </comment>
+    <comment ref="C144" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ما فائدة هذا الوسم في وجود PV_Pass-aAat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C146" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>هذا وسم غير منطقي إذ ليس من مبني للمجهول يختص بضمير الرفع المستتر المذكر دون غيره من مستتر أو متصل، فأجذعه الثمانية تناسب PV_Pass-aAat.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C153" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>هذا وسم غير منطقي إذ ليس من مبني للمجهول يختص بضمير الرفع المستتر المذكر دون غيره من مستتر أو متصل، فأجذعه الثمانية تناسب PV_Pass-aAat.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>omar</author>
+  </authors>
+  <commentList>
+    <comment ref="A15" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>omar:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+ملاحظة خاطئة</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="531">
   <si>
     <t>Nprop</t>
   </si>
@@ -710,90 +786,12 @@
     <t>Freq</t>
   </si>
   <si>
-    <t>فعل ماضٍ معتلّ الآخر متعدٍّ - آخره المعلول محذوف من الجذع كما لا تعوضه اللواحق</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ معتلّ الآخر لازم - آخره المعلول محذوف من الجذع كما لا تعوضه اللواحق</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ معتلّ الآخر أو مهموزه متعدٍّ - الجذع: للفعل مهموز الآخر الهمزة على واو، وللفعل معتل الآخر يُحذف حرف العلة من الجذع</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ معتلّ الآخر أو مهموزه لازم - الجذع: للفعل مهموز الآخر الهمزة على واو، وللفعل معتل الآخر يُحذف حرف العلة من الجذع</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ معتلّ الآخر أو مهموزه متعدٍّ مبنيّ للمجهول - الجذع: للفعل مهموز الآخر الهمزة على واو، وللفعل معتل الآخر يُحذف حرف العلة من الجذع</t>
-  </si>
-  <si>
-    <t>في التقسيم ثغرة كبيرة، وهي أنه لا يفرق من المبنيّ للمجهول بين اللازم والمتعدي، بل إنه يعتبر كلّ مبنيّ للمجهول لازماً، وعليه لن يتعرف كلمات مثل "قُتِلنا" و سيتعرف كلمات خاطئة مثل "ذُهِبنا"</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ معتلّ الآخر بألف أصلها ياء (تُكتب مقصورة) - الجذع هو الفعل ذاته</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ معتلّ الآخر بألف أصلها واو (تُكتب ممدودة) - الجذع هو الفعل ذاته</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ معتلّ الآخر بألف أصلها ياء (تُكتب مقصورة) - في الجذع تعود الألف ياء ليتصل بالضمائر المتصلة</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ مهموز الآخر لازم - الجذع هو الفعل الماضي ذاته</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ مهموز الآخر متعدٍّ - الجذع هو الفعل الماضي ذاته</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ آخره تاء متعدٍّ - الجذع هو الفعل الماضي ذاته</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ آخره تاء لازم - الجذع هو الفعل الماضي ذاته</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ آخره تاء ساكن ما قبلها متعدٍّ - الجذع هو الفعل الماضي ذاته</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ آخره تاء ساكن ما قبلها لازم - الجذع هو الفعل الماضي ذاته</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ معتلّ الآخر بألف أصلها ياء (تُكتب مقصورة) - في الجذع تُقلب الألف المقصورة ألفا ممدودة ليتصل بما يناسبه من الضمائر</t>
-  </si>
-  <si>
     <t>عدد عشري من 20 إلى 90</t>
   </si>
   <si>
     <t>اسم علم</t>
   </si>
   <si>
-    <t>فعل ماضٍ معتلّ الآخر بألف أصلها ياء أو صحيح الآخر بياء متحرّك ما قبل آخره متعدٍّ مبنيّ للمجهول (الفرق بين هذين النوعين غير واضح PV_Pass-a و PV_Pass-aAat) (حالة خاصة أُهمِلت هي الأفعال الماضية المنتهية بنون مشددة مثل "سَنَّ")</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ صحيح متحرّك ما قبل آخره متعدٍّ</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ صحيح متحرّك ما قبل آخره لازم</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ صحيح متحرّك ما قبل آخره متعدٍّ مبنيّ للمجهول</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ آخره نون متعدٍّ - الجذع هو الفعل الماضي ذاته</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ آخره نون لازم - الجذع هو الفعل الماضي ذاته</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ آخره نون متعدٍّ مبنيّ للمجهول - الجذع هو الفعل الماضي ذاته (ينقص هذا النوع لاحق هو نا الفاعلين، فلن يتعرف "لُعِنّا")</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ آخره نون ساكن ما قبل آخره متعدٍّ - الجذع مفكوك التضعيف إن وُجد، محذوف العين إن كان مُعتلّا، وكل ذلك لمنع التقاء الساكنين عند اتصال الفعل بالضمائر المتصلة</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ آخره نون ساكن ما قبل آخره لازم - الجذع مفكوك التضعيف إن وُجد، محذوف العين إن كان مُعتلّا، وكل ذلك لمنع التقاء الساكنين عند اتصال الفعل بالضمائر المتصلة</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ معتلّ الآخر بألف أصلها ياء أو صحيح الآخر بياء، متحرّك ما قبل آخره، متعدٍّ، مبنيّ للمجهول ("أُرِيَه" غير مشمول)</t>
-  </si>
-  <si>
     <t>معناه</t>
   </si>
   <si>
@@ -827,27 +825,9 @@
     <t>لا يشمل ما آخره تاء أو نون أو همز وفي نفس الوقت معلول ما قبل آخره مثل بان وبات وباء، فكيف يتعرف "بنّا" و"بتُّ" و"بؤت"؟</t>
   </si>
   <si>
-    <t>فعل ماضٍ آخره إما ألف علة أصلها ياء أو ياء صحيحة، متحرّك ما قبل آخره، مبنيّ للمجهول، متعدٍّ - في الجذع قُلبت ألف العلة ياء</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ آخره ياء صحيحة، متحرّك ما قبل آخره، مبنيّ للمعلوم، لازم - الجذع هو الفعل ذاته</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ آخره ياء صحيحة، متحرّك ما قبل آخره، مبنيّ للمعلوم، متعدّ - الجذع هو الفعل ذاته</t>
-  </si>
-  <si>
     <t>PV_C_Pass وسم به ثلاثة أفعال، اثنان منهما بهما خطأ ؛ هو أن عين الفعل مفتوحة ويجب أن تُكسر</t>
   </si>
   <si>
-    <t>فعل ماضٍ صحيح الآخر، ساكن ما قبل آخره، متعدٍّ - الجذع مفكوك التضعيف إن وُجد، محذوف العين إن كان مُعتلّا، وذلك لمنع التقاء الساكنين فيجوزَ اتصال الفعل بضمائر المتكلم والمخاطب دون الغائب</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ صحيح الآخر، ساكن ما قبل آخره، لازم - الجذع مفكوك التضعيف إن وُجد، محذوف العين إن كان مُعتلّا، وذلك لمنع التقاء الساكنين فيجوزَ اتصال الفعل بضمائر المتكلم والمخاطب دون الغائب</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ صحيح الآخر، ساكن ما قبل آخره، مبنيّ للمجهول، متعدٍّ - الجذع مفكوك التضعيف إن وُجد، أو محذوف العين إن كان مُعتلّا، وذلك لمنع التقاء الساكنين فيجوزَ اتصال الفعل بضمائر المتكلم والمخاطب دون الغائب</t>
-  </si>
-  <si>
     <t>اسم صحيح الآخر، يبدأ بلام، مذكر، يجمع بجمع المذكر السالم</t>
   </si>
   <si>
@@ -1193,25 +1173,10 @@
     <t>أفعال الأمر تحتاج عناية خاصة</t>
   </si>
   <si>
-    <t>فعل ماضٍ، معتلّ العين (ما قبل الآخر) أو مضاعف (العين واللام)، متعدٍّ، مبنيّ للمجهول - عينه المعلول لا يسمح بإلحاق ضمائر المتكلم والمخاطب منعا لالتقاء الساكنين، ويسمح بضمائر الغائب</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ، معتلّ العين (ما قبل الآخر) أو مضاعف (العين واللام)، لازم، مبنيّ للمعلوم - الجذع هو الفعل ذاته</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ، معتلّ العين (ما قبل الآخر) أو مضاعف (العين واللام)، متعدٍّ، مبنيّ للمعلوم - الجذع هو الفعل ذاته</t>
-  </si>
-  <si>
     <t>فعل أمر، متعدٍّ، صحيح العين، صحيح الآخر (اللام)، مبنيّ على السكون - الجذع على صورة الفعل حين يكون تقدير فاعله "أنتَ"، لا حركة على آخره</t>
   </si>
   <si>
     <t>فعل أمر، لازم، صحيح العين، صحيح الآخر (اللام)، مبنيّ على السكون - الجذع على صورة الفعل حين يكون تقدير فاعله "أنتَ"، لا حركة على آخره</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ مهموز الآخر لازم - الجذع: تُبدل الهمزة ألف مد (آ)</t>
-  </si>
-  <si>
-    <t>فعل ماضٍ مهموز الآخر متعدٍّ - الجذع: تُبدل الهمزة ألف مد (آ) (يسبب هذا النوع كلاحقه خطأ إملائيا، وذلك أنه متوافق مع لواحق تبدأ بألف فيصبح شكل الكلمة "قرآاه" بدل "قرآه")</t>
   </si>
   <si>
     <t>IV_need-Pref-| لأفعال مثل آكل ولكنه لا يغطي الأفعال البدئة بهمزة المنتهية بنون، لأنه أصلا ما عنده نون توكيد وأما نون النسوة فلا تلحق أفعل</t>
@@ -1958,6 +1923,132 @@
   <si>
     <t>اِخْتَفَت,مَقُت</t>
   </si>
+  <si>
+    <t>("أُرِيَه" غير مشمول)</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، معتلّ العين أو مضعّف العين، متعدٍّ، مبنيّ للمعلوم - الجذع هو الفعل ذاته</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، معتلّ العين أو مضعّف العين، لازم، مبنيّ للمعلوم - الجذع هو الفعل ذاته</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، معتلّ العين أو مضعّف العين، متعدٍّ، مبنيّ للمجهول - عينه المعلول لا يسمح بإلحاق ضمائر المتكلم والمخاطب منعا لالتقاء الساكنين، ويسمح بضمائر الغائب</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، معتلّ الآخر أو مهموزه، متعدٍّ مبنيّ للمجهول - الجذع: للفعل مهموز الآخر الهمزة على واو، وللفعل معتل الآخر يُحذف حرف العلة من الجذع</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، صحيح متحرّك ما قبل آخره متعدٍّ</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، معتلّ الآخر بألف أصلها ياء (تُكتب مقصورة) - الجذع هو الفعل ذاته</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، معتلّ الآخر بألف أصلها واو (تُكتب ممدودة) - الجذع هو الفعل ذاته</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، معتلّ الآخر بألف أصلها ياء (تُكتب مقصورة) - في الجذع تعود الألف ياء ليتصل بالضمائر المتصلة</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، صحيح الآخر، ساكن ما قبل آخره، متعدٍّ - الجذع مفكوك التضعيف إن وُجد، محذوف العين إن كان مُعتلّا، وذلك لمنع التقاء الساكنين فيجوزَ اتصال الفعل بضمائر المتكلم والمخاطب دون الغائب</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، صحيح الآخر، ساكن ما قبل آخره، لازم - الجذع مفكوك التضعيف إن وُجد، محذوف العين إن كان مُعتلّا، وذلك لمنع التقاء الساكنين فيجوزَ اتصال الفعل بضمائر المتكلم والمخاطب دون الغائب</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، صحيح الآخر، ساكن ما قبل آخره، مبنيّ للمجهول، متعدٍّ - الجذع مفكوك التضعيف إن وُجد، أو محذوف العين إن كان مُعتلّا، وذلك لمنع التقاء الساكنين فيجوزَ اتصال الفعل بضمائر المتكلم والمخاطب دون الغائب</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، آخره نون ساكن ما قبل آخره متعدٍّ - الجذع مفكوك التضعيف إن وُجد، محذوف العين إن كان مُعتلّا، وكل ذلك لمنع التقاء الساكنين عند اتصال الفعل بالضمائر المتصلة</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، آخره نون ساكن ما قبل آخره لازم - الجذع مفكوك التضعيف إن وُجد، محذوف العين إن كان مُعتلّا، وكل ذلك لمنع التقاء الساكنين عند اتصال الفعل بالضمائر المتصلة</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، آخره تاء ساكن ما قبلها متعدٍّ - الجذع مفكوك التضعيف إن وُجد، محذوف العين إن كان مُعتلّا، مُهيّأ لاتصال بتاء المتكلم مدغمة في التاء الأصلية</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، آخره تاء ساكن ما قبلها لازم - الجذع مفكوك التضعيف إن وُجد، محذوف العين إن كان مُعتلّا، مُهيّأ لاتصال بتاء المتكلم مدغمة في التاء الأصلية</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، معتلّ الآخر بألف أصلها ياء (تُكتب مقصورة) - في الجذع تُقلب الألف المقصورة ألفا ممدودة ليتصل بما يناسبه من الضمائر</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، صحيح متحرّك ما قبل آخره لازم</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، معتلّ الآخر بألف أصلها ياء أو صحيح الآخر بياء، متحرّك ما قبل آخره، متعدٍّ، مبنيّ للمجهول ("أُرِيَه" غير مشمول)</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، مهموز الآخر، لازم - الجذع: تُبدل الهمزة ألف مد (آ)</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، مهموز الآخر، متعدٍّ - الجذع هو الفعل الماضي ذاته</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، مهموز الآخر، لازم - الجذع هو الفعل الماضي ذاته</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، آخره نون، متعدٍّ - الجذع هو الفعل الماضي ذاته</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، آخره نون، لازم - الجذع هو الفعل الماضي ذاته</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، آخره تاء، متعدٍّ - الجذع هو الفعل الماضي ذاته</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، آخره تاء، لازم - الجذع هو الفعل الماضي ذاته</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، آخره نون، متعدٍّ مبنيّ للمجهول - الجذع هو الفعل الماضي ذاته</t>
+  </si>
+  <si>
+    <t>PV-n_Pass ينقص هذا النوع لاحق هو نا الفاعلين، فلن يتعرف "لُعِنّا" و"غُبِنّا"</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، مهموز الآخر، متعدٍّ - الجذع: تُبدل الهمزة ألف مد (آ)</t>
+  </si>
+  <si>
+    <t>PV-|, PV-|_intr: يسبب هذان النوعان خطأ إملائيا، وذلك أنهما متوافقان مع لواحق تبدأ بألف فيصبح شكل الكلمة "قرآاه" بدل "قرآه"</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، معتلّ الآخر أو معتل العين، متعدٍّ، مبنيّ للمجهول</t>
+  </si>
+  <si>
+    <t>حالة خاصة أُهمِلت هي الأفعال الماضية المنتهية بنون مشددة مثل "سَنَّ"</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، آخره ألف علّة (مقصورة أو ممدودة)، متعدٍّ - آخره المعلول محذوف من الجذع كما لا تعوضه اللواحق</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، آخره ألف علّة (مقصورة أو ممدودة)، لازم - آخره المعلول محذوف من الجذع كما لا تعوضه اللواحق</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، آخره همزة أو ياء، متعدٍّ - الجذع: للفعل مهموز الآخر الهمزة على واو، وللفعل معتل الآخر يُحذف حرف العلة من الجذع</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، آخره همزة أو ياء، لازم - الجذع: للفعل مهموز الآخر الهمزة على واو، وللفعل معتل الآخر يُحذف حرف العلة من الجذع</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، آخره ياء، متحرّك ما قبل آخره، مبنيّ للمعلوم، متعدّ - الجذع هو الفعل ذاته</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، آخره ياء، متحرّك ما قبل آخره، مبنيّ للمعلوم، لازم - الجذع هو الفعل ذاته</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، آخره إما ألف علة أصلها ياء أو ياء، متحرّك ما قبل آخره، مبنيّ للمجهول، متعدٍّ - في الجذع قُلبت ألف العلة ياء</t>
+  </si>
+  <si>
+    <t>فعل ماضٍ، صحيح، متحرّك ما قبل آخره، متعدٍّ، مبنيّ للمجهول</t>
+  </si>
+  <si>
+    <t>في التقسيم ثغرة كبيرة، وهي أنه لا يفرق من المبنيّ للمجهول بين اللازم والمتعدي، بل إنه يعتبر كلّ مبنيّ للمجهول متعدياً، وعليه سيتعرف كلمات خاطئة مثل "ذُهِبنا"</t>
+  </si>
+  <si>
+    <t>لا اعتبار لاتصال ألف الاثنين بقعل ماض معتل الآخر بألف أصلها واو مثل سما سَمَوَا</t>
+  </si>
 </sst>
 </file>
 
@@ -1970,6 +2061,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="178"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2202,12 +2300,6 @@
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-    </font>
-    <font>
-      <b/>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -2215,7 +2307,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2431,6 +2523,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -2574,69 +2672,69 @@
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2645,83 +2743,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="35" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2771,6 +2875,72 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
     <mruColors>
       <color rgb="FFADFD77"/>
     </mruColors>
@@ -2786,7 +2956,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C0C0C0"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -3077,7 +3247,7 @@
         <v>159</v>
       </c>
       <c r="B1" t="s">
-        <v>379</v>
+        <v>342</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3546,11 +3716,11 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:K166"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B150" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="C155" sqref="C155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5"/>
@@ -3574,10 +3744,10 @@
         <v>160</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>339</v>
+        <v>302</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>380</v>
+        <v>343</v>
       </c>
       <c r="E1" s="37"/>
       <c r="F1"/>
@@ -3595,10 +3765,10 @@
         <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>325</v>
+        <v>290</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>381</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="45">
@@ -3609,10 +3779,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>318</v>
+        <v>286</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>382</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="45">
@@ -3623,10 +3793,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>326</v>
+        <v>291</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>383</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="67.5">
@@ -3637,7 +3807,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>319</v>
+        <v>287</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="67.5">
@@ -3648,7 +3818,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>320</v>
+        <v>288</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -3789,10 +3959,10 @@
         <v>2878</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>299</v>
+        <v>267</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>384</v>
+        <v>347</v>
       </c>
       <c r="F17" s="22"/>
       <c r="G17" s="22"/>
@@ -3805,10 +3975,10 @@
         <v>350</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>300</v>
+        <v>268</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>385</v>
+        <v>348</v>
       </c>
       <c r="F18" s="22"/>
       <c r="G18" s="22"/>
@@ -3822,10 +3992,10 @@
         <v>8</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>364</v>
+        <v>327</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>386</v>
+        <v>349</v>
       </c>
       <c r="F19" s="22"/>
       <c r="G19" s="22"/>
@@ -3839,10 +4009,10 @@
         <v>526</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>301</v>
+        <v>269</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>387</v>
+        <v>350</v>
       </c>
       <c r="F20" s="22"/>
       <c r="G20" s="22"/>
@@ -3855,7 +4025,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>278</v>
+        <v>246</v>
       </c>
       <c r="F21" s="22"/>
       <c r="G21" s="22"/>
@@ -3869,10 +4039,10 @@
         <v>393</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>356</v>
+        <v>319</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>388</v>
+        <v>351</v>
       </c>
       <c r="E22"/>
       <c r="F22" s="22"/>
@@ -3888,10 +4058,10 @@
         <v>10</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>374</v>
+        <v>337</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>389</v>
+        <v>352</v>
       </c>
       <c r="E23"/>
       <c r="F23" s="22"/>
@@ -3906,10 +4076,10 @@
         <v>309</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>375</v>
+        <v>338</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>390</v>
+        <v>353</v>
       </c>
       <c r="E24"/>
       <c r="G24" s="22"/>
@@ -3923,10 +4093,10 @@
         <v>640</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>358</v>
+        <v>321</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>391</v>
+        <v>354</v>
       </c>
       <c r="E25"/>
       <c r="G25" s="22"/>
@@ -3941,10 +4111,10 @@
         <v>16</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>365</v>
+        <v>328</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>392</v>
+        <v>355</v>
       </c>
       <c r="E26"/>
       <c r="G26" s="22"/>
@@ -3958,10 +4128,10 @@
         <v>314</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>357</v>
+        <v>320</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>393</v>
+        <v>356</v>
       </c>
       <c r="E27"/>
       <c r="G27" s="22"/>
@@ -3974,10 +4144,10 @@
         <v>1</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>278</v>
+        <v>246</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>394</v>
+        <v>357</v>
       </c>
       <c r="E28"/>
       <c r="G28" s="22"/>
@@ -3992,10 +4162,10 @@
         <v>269</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>359</v>
+        <v>322</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>395</v>
+        <v>358</v>
       </c>
       <c r="E29"/>
       <c r="G29" s="22"/>
@@ -4010,10 +4180,10 @@
         <v>6</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>366</v>
+        <v>329</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>396</v>
+        <v>359</v>
       </c>
       <c r="E30"/>
       <c r="G30" s="22"/>
@@ -4026,10 +4196,10 @@
         <v>364</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>363</v>
+        <v>326</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>397</v>
+        <v>360</v>
       </c>
       <c r="E31"/>
       <c r="G31" s="22"/>
@@ -4042,10 +4212,10 @@
         <v>1</v>
       </c>
       <c r="C32" s="35" t="s">
-        <v>360</v>
+        <v>323</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>398</v>
+        <v>361</v>
       </c>
       <c r="E32"/>
       <c r="F32" s="22"/>
@@ -4060,7 +4230,7 @@
         <v>1</v>
       </c>
       <c r="C33" s="35" t="s">
-        <v>361</v>
+        <v>324</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33"/>
@@ -4076,10 +4246,10 @@
         <v>690</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>311</v>
+        <v>279</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>399</v>
+        <v>362</v>
       </c>
       <c r="E34"/>
       <c r="F34" s="22"/>
@@ -4094,10 +4264,10 @@
         <v>228</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>400</v>
+        <v>363</v>
       </c>
       <c r="E35"/>
       <c r="F35" s="22"/>
@@ -4112,10 +4282,10 @@
         <v>12</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>401</v>
+        <v>364</v>
       </c>
       <c r="E36"/>
       <c r="F36" s="22"/>
@@ -4129,10 +4299,10 @@
         <v>118</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>314</v>
+        <v>282</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>402</v>
+        <v>365</v>
       </c>
       <c r="E37"/>
       <c r="F37" s="22"/>
@@ -4147,10 +4317,10 @@
         <v>189</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>315</v>
+        <v>283</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>403</v>
+        <v>366</v>
       </c>
       <c r="E38"/>
       <c r="G38" s="22"/>
@@ -4165,10 +4335,10 @@
         <v>2</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>316</v>
+        <v>284</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>404</v>
+        <v>367</v>
       </c>
       <c r="E39"/>
       <c r="G39" s="22"/>
@@ -4183,10 +4353,10 @@
         <v>4</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>317</v>
+        <v>285</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>405</v>
+        <v>368</v>
       </c>
       <c r="E40"/>
       <c r="G40" s="22"/>
@@ -4201,10 +4371,10 @@
         <v>150</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>303</v>
+        <v>271</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>406</v>
+        <v>369</v>
       </c>
       <c r="E41"/>
       <c r="G41" s="22"/>
@@ -4219,10 +4389,10 @@
         <v>2</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>304</v>
+        <v>272</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>407</v>
+        <v>370</v>
       </c>
       <c r="E42"/>
     </row>
@@ -4235,7 +4405,7 @@
       </c>
       <c r="C43" s="26"/>
       <c r="D43" s="2" t="s">
-        <v>408</v>
+        <v>371</v>
       </c>
       <c r="E43"/>
       <c r="F43" s="22"/>
@@ -4251,10 +4421,10 @@
         <v>1439</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>370</v>
+        <v>333</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>409</v>
+        <v>372</v>
       </c>
       <c r="E44"/>
       <c r="F44" s="22"/>
@@ -4270,10 +4440,10 @@
         <v>121</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>371</v>
+        <v>334</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>410</v>
+        <v>373</v>
       </c>
       <c r="E45"/>
       <c r="H45" s="22"/>
@@ -4288,10 +4458,10 @@
         <v>9</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>298</v>
+        <v>266</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>411</v>
+        <v>374</v>
       </c>
       <c r="E46"/>
       <c r="I46" s="22"/>
@@ -4305,10 +4475,10 @@
         <v>11</v>
       </c>
       <c r="C47" s="26" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>412</v>
+        <v>375</v>
       </c>
       <c r="E47"/>
       <c r="F47" s="22"/>
@@ -4325,10 +4495,10 @@
         <v>130</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>294</v>
+        <v>262</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>413</v>
+        <v>376</v>
       </c>
       <c r="E48"/>
       <c r="F48" s="22"/>
@@ -4339,13 +4509,13 @@
     </row>
     <row r="49" spans="1:10" ht="67.5">
       <c r="A49" s="23" t="s">
-        <v>377</v>
+        <v>340</v>
       </c>
       <c r="B49" s="24">
         <v>0</v>
       </c>
       <c r="C49" s="36" t="s">
-        <v>378</v>
+        <v>341</v>
       </c>
       <c r="E49"/>
       <c r="F49" s="22"/>
@@ -4362,10 +4532,10 @@
         <v>9</v>
       </c>
       <c r="C50" s="26" t="s">
-        <v>295</v>
+        <v>263</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>414</v>
+        <v>377</v>
       </c>
       <c r="E50"/>
       <c r="F50" s="22"/>
@@ -4380,10 +4550,10 @@
         <v>1</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>279</v>
+        <v>247</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>415</v>
+        <v>378</v>
       </c>
       <c r="E51"/>
       <c r="F51" s="22"/>
@@ -4399,10 +4569,10 @@
         <v>670</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>282</v>
+        <v>250</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>416</v>
+        <v>379</v>
       </c>
       <c r="E52"/>
       <c r="F52" s="22"/>
@@ -4418,10 +4588,10 @@
         <v>702</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>283</v>
+        <v>251</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>417</v>
+        <v>380</v>
       </c>
       <c r="E53"/>
       <c r="F53" s="22"/>
@@ -4438,10 +4608,10 @@
         <v>233</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>284</v>
+        <v>252</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>418</v>
+        <v>381</v>
       </c>
       <c r="E54"/>
       <c r="F54" s="22"/>
@@ -4457,10 +4627,10 @@
         <v>2</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>281</v>
+        <v>249</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>419</v>
+        <v>382</v>
       </c>
       <c r="E55"/>
       <c r="F55" s="22"/>
@@ -4477,10 +4647,10 @@
         <v>13</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>420</v>
+        <v>383</v>
       </c>
       <c r="E56"/>
       <c r="F56" s="22"/>
@@ -4495,10 +4665,10 @@
         <v>2</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>280</v>
+        <v>248</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>421</v>
+        <v>384</v>
       </c>
       <c r="E57"/>
       <c r="G57" s="22"/>
@@ -4513,10 +4683,10 @@
         <v>173</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>286</v>
+        <v>254</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>422</v>
+        <v>385</v>
       </c>
       <c r="E58"/>
       <c r="I58" s="22"/>
@@ -4530,10 +4700,10 @@
         <v>199</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>287</v>
+        <v>255</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>423</v>
+        <v>386</v>
       </c>
       <c r="E59"/>
       <c r="F59" s="22"/>
@@ -4549,10 +4719,10 @@
         <v>109</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>276</v>
+        <v>244</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>424</v>
+        <v>387</v>
       </c>
       <c r="E60"/>
       <c r="F60" s="22"/>
@@ -4568,10 +4738,10 @@
         <v>1</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>334</v>
+        <v>297</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>425</v>
+        <v>388</v>
       </c>
       <c r="E61"/>
       <c r="I61" s="22"/>
@@ -4585,10 +4755,10 @@
         <v>17</v>
       </c>
       <c r="C62" s="20" t="s">
-        <v>335</v>
+        <v>298</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>426</v>
+        <v>389</v>
       </c>
       <c r="E62"/>
       <c r="I62" s="22"/>
@@ -4602,10 +4772,10 @@
         <v>116</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>336</v>
+        <v>299</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>427</v>
+        <v>390</v>
       </c>
       <c r="E63"/>
       <c r="J63" s="22"/>
@@ -4618,10 +4788,10 @@
         <v>1</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>337</v>
+        <v>300</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>428</v>
+        <v>391</v>
       </c>
       <c r="E64"/>
       <c r="I64" s="22"/>
@@ -4635,10 +4805,10 @@
         <v>1</v>
       </c>
       <c r="C65" s="18" t="s">
-        <v>338</v>
+        <v>301</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>429</v>
+        <v>392</v>
       </c>
       <c r="E65"/>
       <c r="I65" s="22"/>
@@ -4652,10 +4822,10 @@
         <v>6</v>
       </c>
       <c r="C66" s="20" t="s">
-        <v>355</v>
+        <v>318</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>430</v>
+        <v>393</v>
       </c>
       <c r="E66"/>
       <c r="I66" s="22"/>
@@ -4663,13 +4833,13 @@
     </row>
     <row r="67" spans="1:10" s="21" customFormat="1" ht="90">
       <c r="A67" s="23" t="s">
-        <v>341</v>
+        <v>304</v>
       </c>
       <c r="B67" s="24">
         <v>0</v>
       </c>
       <c r="C67" s="25" t="s">
-        <v>342</v>
+        <v>305</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67"/>
@@ -4678,13 +4848,13 @@
     </row>
     <row r="68" spans="1:10" s="21" customFormat="1" ht="90">
       <c r="A68" s="23" t="s">
-        <v>343</v>
+        <v>306</v>
       </c>
       <c r="B68" s="24">
         <v>0</v>
       </c>
       <c r="C68" s="25" t="s">
-        <v>345</v>
+        <v>308</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68"/>
@@ -4693,13 +4863,13 @@
     </row>
     <row r="69" spans="1:10" s="21" customFormat="1" ht="90">
       <c r="A69" s="23" t="s">
-        <v>340</v>
+        <v>303</v>
       </c>
       <c r="B69" s="24">
         <v>0</v>
       </c>
       <c r="C69" s="25" t="s">
-        <v>346</v>
+        <v>309</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69"/>
@@ -4711,13 +4881,13 @@
     </row>
     <row r="70" spans="1:10" s="21" customFormat="1" ht="90">
       <c r="A70" s="23" t="s">
-        <v>344</v>
+        <v>307</v>
       </c>
       <c r="B70" s="24">
         <v>0</v>
       </c>
       <c r="C70" s="25" t="s">
-        <v>347</v>
+        <v>310</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70"/>
@@ -4733,10 +4903,10 @@
         <v>2394</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>330</v>
+        <v>293</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>431</v>
+        <v>394</v>
       </c>
       <c r="E71"/>
       <c r="F71" s="22"/>
@@ -4753,10 +4923,10 @@
         <v>93</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>272</v>
+        <v>240</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>432</v>
+        <v>395</v>
       </c>
       <c r="E72"/>
       <c r="F72" s="22"/>
@@ -4773,10 +4943,10 @@
         <v>162</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>292</v>
+        <v>260</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>433</v>
+        <v>396</v>
       </c>
       <c r="E73"/>
       <c r="F73" s="22"/>
@@ -4793,10 +4963,10 @@
         <v>90</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>291</v>
+        <v>259</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>434</v>
+        <v>397</v>
       </c>
       <c r="E74"/>
       <c r="F74" s="22"/>
@@ -4813,10 +4983,10 @@
         <v>8</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>290</v>
+        <v>258</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>435</v>
+        <v>398</v>
       </c>
       <c r="E75"/>
       <c r="F75" s="22"/>
@@ -4831,10 +5001,10 @@
         <v>2</v>
       </c>
       <c r="C76" s="18" t="s">
-        <v>289</v>
+        <v>257</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>436</v>
+        <v>399</v>
       </c>
       <c r="E76"/>
       <c r="F76" s="22"/>
@@ -4850,10 +5020,10 @@
         <v>30</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>264</v>
+        <v>232</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>437</v>
+        <v>400</v>
       </c>
       <c r="E77"/>
     </row>
@@ -4865,10 +5035,10 @@
         <v>159</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>263</v>
+        <v>231</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>438</v>
+        <v>401</v>
       </c>
       <c r="E78"/>
     </row>
@@ -4880,10 +5050,10 @@
         <v>8818</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>253</v>
+        <v>221</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>439</v>
+        <v>402</v>
       </c>
       <c r="E79"/>
     </row>
@@ -4895,10 +5065,10 @@
         <v>730</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>259</v>
+        <v>227</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>440</v>
+        <v>403</v>
       </c>
       <c r="E80"/>
     </row>
@@ -4910,10 +5080,10 @@
         <v>12</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>261</v>
+        <v>229</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>441</v>
+        <v>404</v>
       </c>
       <c r="E81"/>
     </row>
@@ -4925,10 +5095,10 @@
         <v>1787</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>257</v>
+        <v>225</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>442</v>
+        <v>405</v>
       </c>
       <c r="E82"/>
     </row>
@@ -4940,10 +5110,10 @@
         <v>8</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>258</v>
+        <v>226</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>443</v>
+        <v>406</v>
       </c>
       <c r="E83"/>
     </row>
@@ -4955,10 +5125,10 @@
         <v>210</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>252</v>
+        <v>220</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>444</v>
+        <v>407</v>
       </c>
       <c r="E84"/>
     </row>
@@ -4970,10 +5140,10 @@
         <v>39</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>250</v>
+        <v>218</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>445</v>
+        <v>408</v>
       </c>
       <c r="E85"/>
     </row>
@@ -4985,10 +5155,10 @@
         <v>24</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>249</v>
+        <v>217</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>446</v>
+        <v>409</v>
       </c>
       <c r="E86"/>
     </row>
@@ -5000,10 +5170,10 @@
         <v>3328</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>247</v>
+        <v>215</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>447</v>
+        <v>410</v>
       </c>
       <c r="E87"/>
     </row>
@@ -5015,10 +5185,10 @@
         <v>75</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>248</v>
+        <v>216</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>448</v>
+        <v>411</v>
       </c>
       <c r="E88"/>
     </row>
@@ -5030,10 +5200,10 @@
         <v>1595</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>246</v>
+        <v>214</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>449</v>
+        <v>412</v>
       </c>
       <c r="E89"/>
     </row>
@@ -5045,10 +5215,10 @@
         <v>31</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>245</v>
+        <v>213</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>450</v>
+        <v>413</v>
       </c>
       <c r="E90"/>
     </row>
@@ -5060,10 +5230,10 @@
         <v>76</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>244</v>
+        <v>212</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>451</v>
+        <v>414</v>
       </c>
       <c r="E91"/>
     </row>
@@ -5075,10 +5245,10 @@
         <v>128</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>242</v>
+        <v>210</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>452</v>
+        <v>415</v>
       </c>
       <c r="E92"/>
     </row>
@@ -5090,10 +5260,10 @@
         <v>146</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>243</v>
+        <v>211</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>453</v>
+        <v>416</v>
       </c>
       <c r="E93"/>
     </row>
@@ -5105,10 +5275,10 @@
         <v>5597</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>238</v>
+        <v>206</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>454</v>
+        <v>417</v>
       </c>
       <c r="E94"/>
     </row>
@@ -5120,10 +5290,10 @@
         <v>82</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>239</v>
+        <v>207</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>455</v>
+        <v>418</v>
       </c>
       <c r="E95"/>
     </row>
@@ -5135,10 +5305,10 @@
         <v>829</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>456</v>
+        <v>419</v>
       </c>
       <c r="E96"/>
     </row>
@@ -5150,10 +5320,10 @@
         <v>7</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>457</v>
+        <v>420</v>
       </c>
       <c r="E97"/>
     </row>
@@ -5165,10 +5335,10 @@
         <v>3808</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>458</v>
+        <v>421</v>
       </c>
       <c r="E98"/>
     </row>
@@ -5180,10 +5350,10 @@
         <v>2482</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>459</v>
+        <v>422</v>
       </c>
       <c r="E99"/>
     </row>
@@ -5195,10 +5365,10 @@
         <v>120</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>235</v>
+        <v>203</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>460</v>
+        <v>423</v>
       </c>
       <c r="E100"/>
     </row>
@@ -5210,10 +5380,10 @@
         <v>84</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>461</v>
+        <v>424</v>
       </c>
       <c r="E101"/>
     </row>
@@ -5225,10 +5395,10 @@
         <v>1928</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>462</v>
+        <v>425</v>
       </c>
       <c r="E102"/>
     </row>
@@ -5240,10 +5410,10 @@
         <v>38</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>463</v>
+        <v>426</v>
       </c>
       <c r="E103"/>
     </row>
@@ -5255,10 +5425,10 @@
         <v>1726</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>464</v>
+        <v>427</v>
       </c>
       <c r="E104"/>
     </row>
@@ -5270,10 +5440,10 @@
         <v>39</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>465</v>
+        <v>428</v>
       </c>
       <c r="E105"/>
     </row>
@@ -5285,10 +5455,10 @@
         <v>1495</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>222</v>
+        <v>190</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>466</v>
+        <v>429</v>
       </c>
       <c r="E106"/>
     </row>
@@ -5300,10 +5470,10 @@
         <v>23</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>227</v>
+        <v>195</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>467</v>
+        <v>430</v>
       </c>
       <c r="E107"/>
     </row>
@@ -5315,10 +5485,10 @@
         <v>264</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>331</v>
+        <v>294</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>468</v>
+        <v>431</v>
       </c>
       <c r="E108"/>
     </row>
@@ -5330,10 +5500,10 @@
         <v>2485</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>226</v>
+        <v>194</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>469</v>
+        <v>432</v>
       </c>
       <c r="E109"/>
     </row>
@@ -5345,10 +5515,10 @@
         <v>31</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>470</v>
+        <v>433</v>
       </c>
       <c r="E110"/>
     </row>
@@ -5360,10 +5530,10 @@
         <v>2050</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>471</v>
+        <v>434</v>
       </c>
       <c r="E111"/>
     </row>
@@ -5375,10 +5545,10 @@
         <v>19</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>223</v>
+        <v>191</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>472</v>
+        <v>435</v>
       </c>
       <c r="E112"/>
     </row>
@@ -5390,10 +5560,10 @@
         <v>1617</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>473</v>
+        <v>436</v>
       </c>
       <c r="E113"/>
     </row>
@@ -5405,10 +5575,10 @@
         <v>6</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>474</v>
+        <v>437</v>
       </c>
       <c r="E114"/>
     </row>
@@ -5420,10 +5590,10 @@
         <v>818</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>218</v>
+        <v>186</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>475</v>
+        <v>438</v>
       </c>
       <c r="E115"/>
     </row>
@@ -5435,10 +5605,10 @@
         <v>279</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>476</v>
+        <v>439</v>
       </c>
       <c r="E116"/>
     </row>
@@ -5450,10 +5620,10 @@
         <v>27</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>332</v>
+        <v>295</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>477</v>
+        <v>440</v>
       </c>
       <c r="E117"/>
     </row>
@@ -5465,10 +5635,10 @@
         <v>1277</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>211</v>
+        <v>179</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>478</v>
+        <v>441</v>
       </c>
       <c r="E118"/>
     </row>
@@ -5480,10 +5650,10 @@
         <v>27</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>212</v>
+        <v>180</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>479</v>
+        <v>442</v>
       </c>
       <c r="E119"/>
     </row>
@@ -5495,10 +5665,10 @@
         <v>11</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>333</v>
+        <v>296</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>480</v>
+        <v>443</v>
       </c>
       <c r="E120"/>
     </row>
@@ -5510,10 +5680,10 @@
         <v>11</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>213</v>
+        <v>181</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>481</v>
+        <v>444</v>
       </c>
       <c r="E121"/>
     </row>
@@ -5525,10 +5695,10 @@
         <v>1761</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>482</v>
+        <v>445</v>
       </c>
       <c r="E122"/>
     </row>
@@ -5540,10 +5710,10 @@
         <v>46</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>483</v>
+        <v>446</v>
       </c>
       <c r="E123"/>
     </row>
@@ -5555,10 +5725,10 @@
         <v>515</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>216</v>
+        <v>184</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>484</v>
+        <v>447</v>
       </c>
       <c r="E124"/>
     </row>
@@ -5570,10 +5740,10 @@
         <v>2405</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>485</v>
+        <v>448</v>
       </c>
       <c r="E125"/>
     </row>
@@ -5585,10 +5755,10 @@
         <v>9</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>486</v>
+        <v>449</v>
       </c>
       <c r="E126"/>
     </row>
@@ -5600,10 +5770,10 @@
         <v>288</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>208</v>
+        <v>176</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>487</v>
+        <v>450</v>
       </c>
       <c r="E127"/>
     </row>
@@ -5615,10 +5785,10 @@
         <v>2</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>207</v>
+        <v>175</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>488</v>
+        <v>451</v>
       </c>
       <c r="E128"/>
     </row>
@@ -5630,10 +5800,10 @@
         <v>6124</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>180</v>
+        <v>494</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>489</v>
+        <v>452</v>
       </c>
       <c r="E129"/>
     </row>
@@ -5645,10 +5815,10 @@
         <v>1114</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>167</v>
+        <v>495</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>490</v>
+        <v>453</v>
       </c>
       <c r="E130"/>
     </row>
@@ -5660,10 +5830,10 @@
         <v>77</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>168</v>
+        <v>496</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>491</v>
+        <v>454</v>
       </c>
       <c r="E131"/>
     </row>
@@ -5675,10 +5845,10 @@
         <v>1198</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>169</v>
+        <v>497</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>492</v>
+        <v>455</v>
       </c>
       <c r="E132"/>
     </row>
@@ -5690,10 +5860,10 @@
         <v>1183</v>
       </c>
       <c r="C133" s="8" t="s">
-        <v>204</v>
+        <v>498</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>493</v>
+        <v>456</v>
       </c>
       <c r="E133"/>
     </row>
@@ -5705,10 +5875,10 @@
         <v>326</v>
       </c>
       <c r="C134" s="8" t="s">
-        <v>205</v>
+        <v>499</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>494</v>
+        <v>457</v>
       </c>
       <c r="E134"/>
     </row>
@@ -5720,10 +5890,10 @@
         <v>3</v>
       </c>
       <c r="C135" s="8" t="s">
-        <v>206</v>
+        <v>500</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>495</v>
+        <v>458</v>
       </c>
       <c r="E135"/>
     </row>
@@ -5735,10 +5905,10 @@
         <v>53</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>186</v>
+        <v>501</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>496</v>
+        <v>459</v>
       </c>
       <c r="E136"/>
     </row>
@@ -5750,14 +5920,14 @@
         <v>15</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>187</v>
+        <v>502</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>497</v>
+        <v>460</v>
       </c>
       <c r="E137"/>
     </row>
-    <row r="138" spans="1:5">
+    <row r="138" spans="1:5" ht="45">
       <c r="A138" s="7" t="s">
         <v>91</v>
       </c>
@@ -5765,14 +5935,14 @@
         <v>29</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>174</v>
+        <v>503</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>498</v>
+        <v>461</v>
       </c>
       <c r="E138"/>
     </row>
-    <row r="139" spans="1:5" ht="34.5">
+    <row r="139" spans="1:5" ht="45">
       <c r="A139" s="7" t="s">
         <v>92</v>
       </c>
@@ -5780,10 +5950,10 @@
         <v>5</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>175</v>
+        <v>504</v>
       </c>
       <c r="D139" s="2" t="s">
-        <v>499</v>
+        <v>462</v>
       </c>
       <c r="E139"/>
     </row>
@@ -5795,10 +5965,10 @@
         <v>987</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>176</v>
+        <v>505</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>500</v>
+        <v>463</v>
       </c>
       <c r="E140"/>
     </row>
@@ -5810,14 +5980,14 @@
         <v>1880</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>181</v>
+        <v>506</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>501</v>
+        <v>464</v>
       </c>
       <c r="E141"/>
     </row>
-    <row r="142" spans="1:5" ht="45">
+    <row r="142" spans="1:5">
       <c r="A142" s="7" t="s">
         <v>74</v>
       </c>
@@ -5825,10 +5995,10 @@
         <v>40</v>
       </c>
       <c r="C142" s="8" t="s">
-        <v>202</v>
+        <v>525</v>
       </c>
       <c r="D142" s="2" t="s">
-        <v>502</v>
+        <v>465</v>
       </c>
       <c r="E142"/>
     </row>
@@ -5840,10 +6010,10 @@
         <v>46</v>
       </c>
       <c r="C143" s="8" t="s">
-        <v>201</v>
+        <v>526</v>
       </c>
       <c r="D143" s="2" t="s">
-        <v>503</v>
+        <v>466</v>
       </c>
       <c r="E143"/>
     </row>
@@ -5854,11 +6024,11 @@
       <c r="B144" s="4">
         <v>2</v>
       </c>
-      <c r="C144" s="8" t="s">
-        <v>200</v>
+      <c r="C144" s="18" t="s">
+        <v>527</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>504</v>
+        <v>467</v>
       </c>
       <c r="E144"/>
     </row>
@@ -5870,10 +6040,10 @@
         <v>109</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>182</v>
+        <v>528</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>505</v>
+        <v>468</v>
       </c>
       <c r="E145"/>
     </row>
@@ -5884,15 +6054,15 @@
       <c r="B146" s="4">
         <v>8</v>
       </c>
-      <c r="C146" s="2" t="s">
-        <v>188</v>
+      <c r="C146" s="14" t="s">
+        <v>507</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>506</v>
+        <v>469</v>
       </c>
       <c r="E146"/>
     </row>
-    <row r="147" spans="1:5" ht="67.5">
+    <row r="147" spans="1:5" ht="34.5">
       <c r="A147" s="7" t="s">
         <v>114</v>
       </c>
@@ -5900,14 +6070,14 @@
         <v>14</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>179</v>
+        <v>519</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>507</v>
+        <v>470</v>
       </c>
       <c r="E147"/>
     </row>
-    <row r="148" spans="1:5">
+    <row r="148" spans="1:5" ht="45">
       <c r="A148" s="7" t="s">
         <v>33</v>
       </c>
@@ -5915,14 +6085,14 @@
         <v>979</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>161</v>
+        <v>521</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>508</v>
+        <v>471</v>
       </c>
       <c r="E148"/>
     </row>
-    <row r="149" spans="1:5" ht="34.5">
+    <row r="149" spans="1:5" ht="45">
       <c r="A149" s="7" t="s">
         <v>51</v>
       </c>
@@ -5930,14 +6100,14 @@
         <v>205</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>162</v>
+        <v>522</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>509</v>
+        <v>472</v>
       </c>
       <c r="E149"/>
     </row>
-    <row r="150" spans="1:5" ht="45">
+    <row r="150" spans="1:5">
       <c r="A150" s="7" t="s">
         <v>1</v>
       </c>
@@ -5945,14 +6115,14 @@
         <v>1270</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>324</v>
+        <v>490</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>510</v>
+        <v>473</v>
       </c>
       <c r="E150"/>
     </row>
-    <row r="151" spans="1:5" ht="45">
+    <row r="151" spans="1:5">
       <c r="A151" s="7" t="s">
         <v>55</v>
       </c>
@@ -5960,14 +6130,14 @@
         <v>350</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>323</v>
+        <v>491</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>511</v>
+        <v>474</v>
       </c>
       <c r="E151"/>
     </row>
-    <row r="152" spans="1:5" ht="67.5">
+    <row r="152" spans="1:5" ht="45">
       <c r="A152" s="7" t="s">
         <v>108</v>
       </c>
@@ -5975,25 +6145,25 @@
         <v>32</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>322</v>
+        <v>492</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>512</v>
+        <v>475</v>
       </c>
       <c r="E152"/>
     </row>
-    <row r="153" spans="1:5" ht="67.5">
+    <row r="153" spans="1:5" ht="45">
       <c r="A153" s="7" t="s">
         <v>130</v>
       </c>
       <c r="B153" s="4">
         <v>2</v>
       </c>
-      <c r="C153" s="2" t="s">
-        <v>322</v>
+      <c r="C153" s="14" t="s">
+        <v>492</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>513</v>
+        <v>476</v>
       </c>
       <c r="E153"/>
     </row>
@@ -6005,10 +6175,10 @@
         <v>234</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>163</v>
+        <v>523</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>514</v>
+        <v>477</v>
       </c>
       <c r="E154"/>
     </row>
@@ -6020,10 +6190,10 @@
         <v>96</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>164</v>
+        <v>524</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>515</v>
+        <v>478</v>
       </c>
       <c r="E155"/>
     </row>
@@ -6035,14 +6205,14 @@
         <v>1</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>165</v>
+        <v>493</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>516</v>
+        <v>479</v>
       </c>
       <c r="E156"/>
     </row>
-    <row r="157" spans="1:5" ht="45">
+    <row r="157" spans="1:5">
       <c r="A157" s="7" t="s">
         <v>90</v>
       </c>
@@ -6050,10 +6220,10 @@
         <v>152</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>328</v>
+        <v>517</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>517</v>
+        <v>480</v>
       </c>
       <c r="E157"/>
     </row>
@@ -6065,10 +6235,10 @@
         <v>41</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>327</v>
+        <v>508</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>518</v>
+        <v>481</v>
       </c>
       <c r="E158"/>
     </row>
@@ -6080,10 +6250,10 @@
         <v>153</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>171</v>
+        <v>509</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>519</v>
+        <v>482</v>
       </c>
       <c r="E159"/>
     </row>
@@ -6095,10 +6265,10 @@
         <v>41</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>170</v>
+        <v>510</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>520</v>
+        <v>483</v>
       </c>
       <c r="E160"/>
     </row>
@@ -6110,10 +6280,10 @@
         <v>338</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>183</v>
+        <v>511</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>521</v>
+        <v>484</v>
       </c>
       <c r="E161"/>
     </row>
@@ -6125,14 +6295,14 @@
         <v>122</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>184</v>
+        <v>512</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>522</v>
+        <v>485</v>
       </c>
       <c r="E162"/>
     </row>
-    <row r="163" spans="1:5" ht="45">
+    <row r="163" spans="1:5">
       <c r="A163" s="7" t="s">
         <v>131</v>
       </c>
@@ -6140,10 +6310,10 @@
         <v>1</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>185</v>
+        <v>515</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>523</v>
+        <v>486</v>
       </c>
       <c r="E163"/>
     </row>
@@ -6155,10 +6325,10 @@
         <v>119</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>172</v>
+        <v>513</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>524</v>
+        <v>487</v>
       </c>
       <c r="E164"/>
     </row>
@@ -6170,10 +6340,10 @@
         <v>27</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>173</v>
+        <v>514</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>525</v>
+        <v>488</v>
       </c>
       <c r="E165"/>
     </row>
@@ -6205,24 +6375,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>193</v>
+        <v>167</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>190</v>
+        <v>164</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -6233,36 +6403,36 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>240</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>254</v>
+        <v>222</v>
       </c>
       <c r="C4" t="s">
-        <v>255</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>256</v>
+        <v>224</v>
       </c>
       <c r="C5" t="s">
-        <v>262</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>265</v>
+        <v>233</v>
       </c>
       <c r="C6" t="s">
-        <v>266</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>267</v>
+        <v>235</v>
       </c>
       <c r="C7" t="s">
         <v>150</v>
@@ -6270,18 +6440,18 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>268</v>
+        <v>236</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>269</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>270</v>
+        <v>238</v>
       </c>
       <c r="C9" t="s">
-        <v>288</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -6306,153 +6476,153 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="B1" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="30" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="B3" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="31" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="B4" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="32" t="s">
-        <v>203</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="32" t="s">
-        <v>209</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="32" t="s">
-        <v>210</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="20" t="s">
-        <v>353</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="20" t="s">
-        <v>354</v>
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="32" t="s">
-        <v>219</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="32" t="s">
-        <v>260</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="20" t="s">
-        <v>352</v>
+        <v>315</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="33" t="s">
-        <v>271</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="45">
       <c r="A15" s="33" t="s">
-        <v>273</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="20" t="s">
-        <v>274</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="32" t="s">
-        <v>275</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="32" t="s">
-        <v>277</v>
+        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="20" t="s">
-        <v>351</v>
+        <v>314</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="20" t="s">
-        <v>350</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="20" t="s">
-        <v>293</v>
+        <v>261</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="33" t="s">
-        <v>296</v>
+        <v>264</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="20" t="s">
-        <v>307</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="45">
       <c r="A24" s="20" t="s">
-        <v>306</v>
+        <v>274</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="20" t="s">
-        <v>302</v>
+        <v>270</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="20" t="s">
-        <v>305</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="34" t="s">
-        <v>308</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="20" t="s">
-        <v>309</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="67.5">
       <c r="A29" s="20" t="s">
-        <v>349</v>
+        <v>312</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="20" t="s">
-        <v>348</v>
+        <v>311</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="32" t="s">
-        <v>369</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -6464,10 +6634,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6477,70 +6647,97 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="10" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="27" t="s">
-        <v>241</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="45">
       <c r="A3" s="28" t="s">
-        <v>166</v>
+        <v>529</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="29" t="s">
-        <v>251</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="10" t="s">
-        <v>373</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" s="10" t="s">
-        <v>310</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="10" t="s">
-        <v>321</v>
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="30">
       <c r="A8" s="27" t="s">
-        <v>329</v>
+        <v>292</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" s="10" t="s">
-        <v>362</v>
+        <v>325</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="10" t="s">
-        <v>367</v>
+        <v>330</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="45">
       <c r="A11" s="27" t="s">
-        <v>368</v>
+        <v>331</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="45">
       <c r="A12" s="10" t="s">
-        <v>372</v>
+        <v>335</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" s="10" t="s">
-        <v>376</v>
+        <v>339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="27" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="39" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="38" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="10" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="10" t="s">
+        <v>530</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>